<commit_message>
Helper changed when no params before
</commit_message>
<xml_diff>
--- a/test/xlsx/tablas_referencia.xlsx
+++ b/test/xlsx/tablas_referencia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E22DA8BB-5A0E-4341-8E81-16C6280F6655}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5204FD5C-8039-4907-BD13-6709A2E33E51}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8835" activeTab="2" xr2:uid="{44D62DAF-BDC8-487B-86CE-15C7037211D0}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="262">
   <si>
     <t>grado</t>
   </si>
@@ -818,6 +818,9 @@
   </si>
   <si>
     <t xml:space="preserve">Estas posiciones cuentan con políticas  y guías amplias orientadas al cumplimiento de  la misión asignada y dentro de un sentido estratégico.                                          La supervisión es ejercida  por un Consejo  o Corporación de manera amplia sobre los resultados finales tanto de la estrategia como de resultados operacionales.   </t>
+  </si>
+  <si>
+    <t>tipo_id</t>
   </si>
 </sst>
 </file>
@@ -1636,242 +1639,242 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2503,10 +2506,10 @@
       <c r="C2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="106" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="34"/>
+      <c r="E2" s="107"/>
     </row>
     <row r="3" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21">
@@ -2518,10 +2521,10 @@
       <c r="C3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="106" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="34"/>
+      <c r="E3" s="107"/>
     </row>
     <row r="4" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21">
@@ -2533,10 +2536,10 @@
       <c r="C4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="106" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="34"/>
+      <c r="E4" s="107"/>
     </row>
     <row r="5" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="26">
@@ -2548,10 +2551,10 @@
       <c r="C5" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="106" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="34"/>
+      <c r="E5" s="107"/>
     </row>
     <row r="6" spans="1:5" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29">
@@ -2563,10 +2566,10 @@
       <c r="C6" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="106" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="34"/>
+      <c r="E6" s="107"/>
     </row>
     <row r="7" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26">
@@ -2578,10 +2581,10 @@
       <c r="C7" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="106" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="34"/>
+      <c r="E7" s="107"/>
     </row>
     <row r="8" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="31">
@@ -2593,10 +2596,10 @@
       <c r="C8" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="106" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="34"/>
+      <c r="E8" s="107"/>
     </row>
     <row r="9" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
@@ -2608,10 +2611,10 @@
       <c r="C9" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="106" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="34"/>
+      <c r="E9" s="107"/>
     </row>
     <row r="10" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="21">
@@ -2623,546 +2626,521 @@
       <c r="C10" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="106" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="34"/>
+      <c r="E10" s="107"/>
     </row>
     <row r="11" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="21">
         <v>5</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="52" t="s">
+      <c r="D11" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="53"/>
+      <c r="E11" s="105"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="26">
         <v>4</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="52" t="s">
+      <c r="D12" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="53"/>
+      <c r="E12" s="105"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29">
         <v>4</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="52" t="s">
+      <c r="B13" s="109"/>
+      <c r="C13" s="111"/>
+      <c r="D13" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="53"/>
+      <c r="E13" s="105"/>
     </row>
     <row r="14" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="26">
         <v>3</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="52" t="s">
+      <c r="D14" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="53"/>
+      <c r="E14" s="105"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="31">
         <v>3</v>
       </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="52" t="s">
+      <c r="B15" s="37"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="53"/>
+      <c r="E15" s="105"/>
     </row>
     <row r="16" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="29">
         <v>3</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="46" t="s">
+      <c r="C16" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="52" t="s">
+      <c r="D16" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="53"/>
+      <c r="E16" s="105"/>
     </row>
     <row r="17" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="21">
         <v>2</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="52" t="s">
+      <c r="D17" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="53"/>
+      <c r="E17" s="105"/>
     </row>
     <row r="18" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="51">
+      <c r="A18" s="45">
         <v>1</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="50" t="s">
+      <c r="C18" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="52" t="s">
+      <c r="D18" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="53"/>
+      <c r="E18" s="105"/>
     </row>
     <row r="19" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="51">
+      <c r="A19" s="45">
         <v>8</v>
       </c>
-      <c r="B19" s="54" t="s">
+      <c r="B19" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="55" t="s">
+      <c r="C19" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="59" t="s">
+      <c r="D19" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="60"/>
+      <c r="E19" s="101"/>
     </row>
     <row r="20" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="21">
         <v>7</v>
       </c>
-      <c r="B20" s="56" t="s">
+      <c r="B20" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="57" t="s">
+      <c r="C20" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="59" t="s">
+      <c r="D20" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="60"/>
+      <c r="E20" s="101"/>
     </row>
     <row r="21" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="21">
         <v>6</v>
       </c>
-      <c r="B21" s="56" t="s">
+      <c r="B21" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="57" t="s">
+      <c r="C21" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="59" t="s">
+      <c r="D21" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="60"/>
+      <c r="E21" s="101"/>
     </row>
     <row r="22" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="21">
         <v>5</v>
       </c>
-      <c r="B22" s="56" t="s">
+      <c r="B22" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="58" t="s">
+      <c r="C22" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="59" t="s">
+      <c r="D22" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="60"/>
+      <c r="E22" s="101"/>
     </row>
     <row r="23" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="21">
         <v>11</v>
       </c>
-      <c r="B23" s="61" t="s">
+      <c r="B23" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="62" t="s">
+      <c r="C23" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="65" t="s">
+      <c r="D23" s="102" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="66"/>
+      <c r="E23" s="103"/>
     </row>
     <row r="24" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="21">
         <v>10</v>
       </c>
-      <c r="B24" s="63" t="s">
+      <c r="B24" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="64" t="s">
+      <c r="C24" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="65" t="s">
+      <c r="D24" s="102" t="s">
         <v>51</v>
       </c>
-      <c r="E24" s="66"/>
+      <c r="E24" s="103"/>
     </row>
     <row r="25" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="21">
         <v>9</v>
       </c>
-      <c r="B25" s="63" t="s">
+      <c r="B25" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="64" t="s">
+      <c r="C25" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="65" t="s">
+      <c r="D25" s="102" t="s">
         <v>51</v>
       </c>
-      <c r="E25" s="66"/>
+      <c r="E25" s="103"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21">
         <v>9</v>
       </c>
-      <c r="B26" s="67" t="s">
+      <c r="B26" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="68" t="s">
+      <c r="C26" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="75" t="s">
+      <c r="D26" s="98" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="76"/>
+      <c r="E26" s="99"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="51">
+      <c r="A27" s="45">
         <v>8</v>
       </c>
-      <c r="B27" s="69" t="s">
+      <c r="B27" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="70" t="s">
+      <c r="C27" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="75" t="s">
+      <c r="D27" s="98" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="76"/>
+      <c r="E27" s="99"/>
     </row>
     <row r="28" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="21">
         <v>7</v>
       </c>
-      <c r="B28" s="71" t="s">
+      <c r="B28" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="72" t="s">
+      <c r="C28" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="D28" s="75" t="s">
+      <c r="D28" s="98" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="76"/>
+      <c r="E28" s="99"/>
     </row>
     <row r="29" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="21">
         <v>6</v>
       </c>
-      <c r="B29" s="73" t="s">
+      <c r="B29" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="74" t="s">
+      <c r="C29" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="75" t="s">
+      <c r="D29" s="98" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="76"/>
+      <c r="E29" s="99"/>
     </row>
     <row r="30" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="21">
         <v>5</v>
       </c>
-      <c r="B30" s="73" t="s">
+      <c r="B30" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="74" t="s">
+      <c r="C30" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="75" t="s">
+      <c r="D30" s="98" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="76"/>
+      <c r="E30" s="99"/>
     </row>
     <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="31">
         <v>12</v>
       </c>
-      <c r="B31" s="77" t="s">
+      <c r="B31" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="78" t="s">
+      <c r="C31" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="81" t="s">
+      <c r="D31" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="E31" s="82"/>
+      <c r="E31" s="97"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="21">
         <v>11</v>
       </c>
-      <c r="B32" s="79" t="s">
+      <c r="B32" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="80" t="s">
+      <c r="C32" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="81" t="s">
+      <c r="D32" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="E32" s="82"/>
+      <c r="E32" s="97"/>
     </row>
     <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="21">
         <v>10</v>
       </c>
-      <c r="B33" s="79" t="s">
+      <c r="B33" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="C33" s="80" t="s">
+      <c r="C33" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="81" t="s">
+      <c r="D33" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="E33" s="82"/>
+      <c r="E33" s="97"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="21">
         <v>9</v>
       </c>
-      <c r="B34" s="79" t="s">
+      <c r="B34" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="80" t="s">
+      <c r="C34" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="81" t="s">
+      <c r="D34" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="E34" s="82"/>
+      <c r="E34" s="97"/>
     </row>
     <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="21">
         <v>15</v>
       </c>
-      <c r="B35" s="83" t="s">
+      <c r="B35" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="84" t="s">
+      <c r="C35" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="D35" s="90" t="s">
+      <c r="D35" s="94" t="s">
         <v>72</v>
       </c>
-      <c r="E35" s="91"/>
+      <c r="E35" s="95"/>
     </row>
     <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="21">
         <v>14</v>
       </c>
-      <c r="B36" s="85" t="s">
+      <c r="B36" s="69" t="s">
         <v>69</v>
       </c>
-      <c r="C36" s="86" t="s">
+      <c r="C36" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="90" t="s">
+      <c r="D36" s="94" t="s">
         <v>72</v>
       </c>
-      <c r="E36" s="91"/>
+      <c r="E36" s="95"/>
     </row>
     <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="89">
+      <c r="A37" s="73">
         <v>13</v>
       </c>
-      <c r="B37" s="85" t="s">
+      <c r="B37" s="69" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="86" t="s">
+      <c r="C37" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="D37" s="90" t="s">
+      <c r="D37" s="94" t="s">
         <v>72</v>
       </c>
-      <c r="E37" s="91"/>
+      <c r="E37" s="95"/>
     </row>
     <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="31">
         <v>12</v>
       </c>
-      <c r="B38" s="87" t="s">
+      <c r="B38" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="88" t="s">
+      <c r="C38" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="D38" s="90" t="s">
+      <c r="D38" s="94" t="s">
         <v>72</v>
       </c>
-      <c r="E38" s="91"/>
+      <c r="E38" s="95"/>
     </row>
     <row r="39" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="96">
+      <c r="A39" s="78">
         <v>18</v>
       </c>
-      <c r="B39" s="92" t="s">
+      <c r="B39" s="74" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="93" t="s">
+      <c r="C39" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="D39" s="97" t="s">
+      <c r="D39" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="E39" s="98"/>
+      <c r="E39" s="93"/>
     </row>
     <row r="40" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="21">
         <v>17</v>
       </c>
-      <c r="B40" s="94" t="s">
+      <c r="B40" s="76" t="s">
         <v>75</v>
       </c>
-      <c r="C40" s="95" t="s">
+      <c r="C40" s="77" t="s">
         <v>74</v>
       </c>
-      <c r="D40" s="97" t="s">
+      <c r="D40" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="E40" s="98"/>
+      <c r="E40" s="93"/>
     </row>
     <row r="41" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="21">
         <v>16</v>
       </c>
-      <c r="B41" s="94" t="s">
+      <c r="B41" s="76" t="s">
         <v>76</v>
       </c>
-      <c r="C41" s="95" t="s">
+      <c r="C41" s="77" t="s">
         <v>74</v>
       </c>
-      <c r="D41" s="97" t="s">
+      <c r="D41" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="E41" s="98"/>
+      <c r="E41" s="93"/>
     </row>
     <row r="42" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="21">
         <v>15</v>
       </c>
-      <c r="B42" s="94" t="s">
+      <c r="B42" s="76" t="s">
         <v>77</v>
       </c>
-      <c r="C42" s="95" t="s">
+      <c r="C42" s="77" t="s">
         <v>74</v>
       </c>
-      <c r="D42" s="97" t="s">
+      <c r="D42" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="E42" s="98"/>
+      <c r="E42" s="93"/>
     </row>
     <row r="43" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="21">
         <v>14</v>
       </c>
-      <c r="B43" s="94" t="s">
+      <c r="B43" s="76" t="s">
         <v>78</v>
       </c>
-      <c r="C43" s="95" t="s">
+      <c r="C43" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="D43" s="97" t="s">
+      <c r="D43" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="E43" s="98"/>
+      <c r="E43" s="93"/>
     </row>
     <row r="44" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="89">
+      <c r="A44" s="73">
         <v>13</v>
       </c>
-      <c r="B44" s="94" t="s">
+      <c r="B44" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="C44" s="95" t="s">
+      <c r="C44" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="D44" s="97" t="s">
+      <c r="D44" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="E44" s="98"/>
+      <c r="E44" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
@@ -3171,12 +3149,37 @@
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3184,10 +3187,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC65C15-1C40-4251-A583-2703229E8E4D}">
-  <dimension ref="A1:E204"/>
+  <dimension ref="A1:G204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A205" sqref="A205"/>
+    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
+      <selection activeCell="G191" sqref="G191:G204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3195,7 +3198,7 @@
     <col min="4" max="4" width="65" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>82</v>
       </c>
@@ -3211,131 +3214,155 @@
       <c r="E1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="146.25" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="146.25" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>23</v>
       </c>
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="79" t="s">
         <v>86</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="106" t="s">
+      <c r="D2" s="86" t="s">
         <v>93</v>
       </c>
       <c r="E2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>23</v>
       </c>
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="80" t="s">
         <v>87</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="107" t="s">
+      <c r="D3" s="87" t="s">
         <v>94</v>
       </c>
       <c r="E3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>13</v>
       </c>
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="81" t="s">
         <v>88</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="108" t="s">
+      <c r="D4" s="88" t="s">
         <v>95</v>
       </c>
       <c r="E4" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="110.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="110.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>13</v>
       </c>
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="82" t="s">
         <v>89</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="108" t="s">
+      <c r="D5" s="88" t="s">
         <v>96</v>
       </c>
       <c r="E5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="104.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="104.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10</v>
       </c>
-      <c r="B6" s="103" t="s">
+      <c r="B6" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="109" t="s">
+      <c r="D6" s="89" t="s">
         <v>97</v>
       </c>
       <c r="E6" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="136.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="136.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10</v>
       </c>
-      <c r="B7" s="104" t="s">
+      <c r="B7" s="84" t="s">
         <v>91</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="110" t="s">
+      <c r="D7" s="90" t="s">
         <v>98</v>
       </c>
       <c r="E7" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="118.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="118.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10</v>
       </c>
-      <c r="B8" s="105" t="s">
+      <c r="B8" s="85" t="s">
         <v>92</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" s="111" t="s">
+      <c r="D8" s="91" t="s">
         <v>99</v>
       </c>
       <c r="E8" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="169.5" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="153.75" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>26</v>
       </c>
-      <c r="B9" s="99" t="s">
+      <c r="B9" s="79" t="s">
         <v>86</v>
       </c>
       <c r="C9">
@@ -3347,12 +3374,15 @@
       <c r="E9" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>26</v>
       </c>
-      <c r="B10" s="100" t="s">
+      <c r="B10" s="80" t="s">
         <v>87</v>
       </c>
       <c r="C10">
@@ -3364,12 +3394,15 @@
       <c r="E10" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="80.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="80.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>15</v>
       </c>
-      <c r="B11" s="101" t="s">
+      <c r="B11" s="81" t="s">
         <v>88</v>
       </c>
       <c r="C11">
@@ -3381,12 +3414,15 @@
       <c r="E11" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="110.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="110.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>15</v>
       </c>
-      <c r="B12" s="102" t="s">
+      <c r="B12" s="82" t="s">
         <v>89</v>
       </c>
       <c r="C12">
@@ -3398,12 +3434,15 @@
       <c r="E12" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="104.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="104.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="103" t="s">
+      <c r="B13" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C13">
@@ -3415,12 +3454,15 @@
       <c r="E13" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="136.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="136.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="104" t="s">
+      <c r="B14" s="84" t="s">
         <v>91</v>
       </c>
       <c r="C14">
@@ -3432,12 +3474,15 @@
       <c r="E14" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="118.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="118.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>12</v>
       </c>
-      <c r="B15" s="105" t="s">
+      <c r="B15" s="85" t="s">
         <v>92</v>
       </c>
       <c r="C15">
@@ -3449,12 +3494,15 @@
       <c r="E15" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="146.25" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="146.25" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>30</v>
       </c>
-      <c r="B16" s="99" t="s">
+      <c r="B16" s="79" t="s">
         <v>86</v>
       </c>
       <c r="C16">
@@ -3466,12 +3514,15 @@
       <c r="E16" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>30</v>
       </c>
-      <c r="B17" s="100" t="s">
+      <c r="B17" s="80" t="s">
         <v>87</v>
       </c>
       <c r="C17">
@@ -3483,12 +3534,15 @@
       <c r="E17" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="80.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="80.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>19</v>
       </c>
-      <c r="B18" s="101" t="s">
+      <c r="B18" s="81" t="s">
         <v>88</v>
       </c>
       <c r="C18">
@@ -3500,12 +3554,15 @@
       <c r="E18" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="110.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="110.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>19</v>
       </c>
-      <c r="B19" s="102" t="s">
+      <c r="B19" s="82" t="s">
         <v>89</v>
       </c>
       <c r="C19">
@@ -3517,12 +3574,15 @@
       <c r="E19" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="104.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="104.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>15</v>
       </c>
-      <c r="B20" s="103" t="s">
+      <c r="B20" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C20">
@@ -3534,12 +3594,15 @@
       <c r="E20" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="136.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="136.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>15</v>
       </c>
-      <c r="B21" s="104" t="s">
+      <c r="B21" s="84" t="s">
         <v>91</v>
       </c>
       <c r="C21">
@@ -3551,12 +3614,15 @@
       <c r="E21" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="118.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="118.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>15</v>
       </c>
-      <c r="B22" s="105" t="s">
+      <c r="B22" s="85" t="s">
         <v>92</v>
       </c>
       <c r="C22">
@@ -3568,12 +3634,15 @@
       <c r="E22" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="146.25" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="146.25" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>35</v>
       </c>
-      <c r="B23" s="99" t="s">
+      <c r="B23" s="79" t="s">
         <v>86</v>
       </c>
       <c r="C23">
@@ -3585,12 +3654,15 @@
       <c r="E23" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>35</v>
       </c>
-      <c r="B24" s="100" t="s">
+      <c r="B24" s="80" t="s">
         <v>87</v>
       </c>
       <c r="C24">
@@ -3602,12 +3674,15 @@
       <c r="E24" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="80.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="80.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" s="101" t="s">
+      <c r="B25" s="81" t="s">
         <v>88</v>
       </c>
       <c r="C25">
@@ -3619,12 +3694,15 @@
       <c r="E25" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="110.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="110.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>23</v>
       </c>
-      <c r="B26" s="102" t="s">
+      <c r="B26" s="82" t="s">
         <v>89</v>
       </c>
       <c r="C26">
@@ -3636,12 +3714,15 @@
       <c r="E26" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="104.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="104.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>18</v>
       </c>
-      <c r="B27" s="103" t="s">
+      <c r="B27" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C27">
@@ -3653,12 +3734,15 @@
       <c r="E27" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="136.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="136.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>18</v>
       </c>
-      <c r="B28" s="104" t="s">
+      <c r="B28" s="84" t="s">
         <v>91</v>
       </c>
       <c r="C28">
@@ -3670,12 +3754,15 @@
       <c r="E28" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="118.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="118.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>18</v>
       </c>
-      <c r="B29" s="105" t="s">
+      <c r="B29" s="85" t="s">
         <v>92</v>
       </c>
       <c r="C29">
@@ -3687,12 +3774,15 @@
       <c r="E29" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="146.25" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="146.25" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>41</v>
       </c>
-      <c r="B30" s="99" t="s">
+      <c r="B30" s="79" t="s">
         <v>86</v>
       </c>
       <c r="C30">
@@ -3704,12 +3794,15 @@
       <c r="E30" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="71.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>41</v>
       </c>
-      <c r="B31" s="100" t="s">
+      <c r="B31" s="80" t="s">
         <v>87</v>
       </c>
       <c r="C31">
@@ -3721,12 +3814,15 @@
       <c r="E31" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="82.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="80.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>28</v>
       </c>
-      <c r="B32" s="101" t="s">
+      <c r="B32" s="81" t="s">
         <v>88</v>
       </c>
       <c r="C32">
@@ -3738,12 +3834,15 @@
       <c r="E32" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="119.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="110.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>28</v>
       </c>
-      <c r="B33" s="102" t="s">
+      <c r="B33" s="82" t="s">
         <v>89</v>
       </c>
       <c r="C33">
@@ -3755,12 +3854,15 @@
       <c r="E33" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="104.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="104.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>22</v>
       </c>
-      <c r="B34" s="103" t="s">
+      <c r="B34" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C34">
@@ -3772,12 +3874,15 @@
       <c r="E34" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="136.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="136.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>22</v>
       </c>
-      <c r="B35" s="104" t="s">
+      <c r="B35" s="84" t="s">
         <v>91</v>
       </c>
       <c r="C35">
@@ -3789,12 +3894,15 @@
       <c r="E35" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="118.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="118.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>22</v>
       </c>
-      <c r="B36" s="105" t="s">
+      <c r="B36" s="85" t="s">
         <v>92</v>
       </c>
       <c r="C36">
@@ -3806,8 +3914,11 @@
       <c r="E36" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>41</v>
       </c>
@@ -3823,8 +3934,11 @@
       <c r="E37" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>41</v>
       </c>
@@ -3840,8 +3954,11 @@
       <c r="E38" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>28</v>
       </c>
@@ -3857,8 +3974,11 @@
       <c r="E39" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>28</v>
       </c>
@@ -3874,8 +3994,11 @@
       <c r="E40" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>22</v>
       </c>
@@ -3891,8 +4014,11 @@
       <c r="E41" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>22</v>
       </c>
@@ -3908,8 +4034,11 @@
       <c r="E42" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>22</v>
       </c>
@@ -3925,8 +4054,11 @@
       <c r="E43" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>47</v>
       </c>
@@ -3942,8 +4074,11 @@
       <c r="E44" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>47</v>
       </c>
@@ -3959,8 +4094,11 @@
       <c r="E45" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>34</v>
       </c>
@@ -3976,8 +4114,11 @@
       <c r="E46" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>34</v>
       </c>
@@ -3993,8 +4134,11 @@
       <c r="E47" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>27</v>
       </c>
@@ -4010,8 +4154,11 @@
       <c r="E48" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>27</v>
       </c>
@@ -4027,8 +4174,11 @@
       <c r="E49" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G49">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>27</v>
       </c>
@@ -4044,8 +4194,11 @@
       <c r="E50" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G50">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>55</v>
       </c>
@@ -4061,8 +4214,11 @@
       <c r="E51" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>55</v>
       </c>
@@ -4078,8 +4234,11 @@
       <c r="E52" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>41</v>
       </c>
@@ -4095,8 +4254,11 @@
       <c r="E53" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>41</v>
       </c>
@@ -4112,8 +4274,11 @@
       <c r="E54" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>32</v>
       </c>
@@ -4129,8 +4294,11 @@
       <c r="E55" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G55">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>32</v>
       </c>
@@ -4146,8 +4314,11 @@
       <c r="E56" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>32</v>
       </c>
@@ -4163,8 +4334,11 @@
       <c r="E57" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G57">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>63</v>
       </c>
@@ -4180,8 +4354,11 @@
       <c r="E58" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>63</v>
       </c>
@@ -4197,8 +4374,11 @@
       <c r="E59" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>50</v>
       </c>
@@ -4214,8 +4394,11 @@
       <c r="E60" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>50</v>
       </c>
@@ -4231,8 +4414,11 @@
       <c r="E61" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G61">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>39</v>
       </c>
@@ -4248,8 +4434,11 @@
       <c r="E62" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G62">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>39</v>
       </c>
@@ -4265,8 +4454,11 @@
       <c r="E63" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G63">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>39</v>
       </c>
@@ -4282,8 +4474,11 @@
       <c r="E64" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G64">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>73</v>
       </c>
@@ -4299,8 +4494,11 @@
       <c r="E65" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>73</v>
       </c>
@@ -4316,8 +4514,11 @@
       <c r="E66" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>61</v>
       </c>
@@ -4333,8 +4534,11 @@
       <c r="E67" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>61</v>
       </c>
@@ -4350,8 +4554,11 @@
       <c r="E68" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>47</v>
       </c>
@@ -4367,8 +4574,11 @@
       <c r="E69" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>47</v>
       </c>
@@ -4384,8 +4594,11 @@
       <c r="E70" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G70">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>47</v>
       </c>
@@ -4401,8 +4614,11 @@
       <c r="E71" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G71">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>84</v>
       </c>
@@ -4418,8 +4634,11 @@
       <c r="E72" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>84</v>
       </c>
@@ -4435,8 +4654,11 @@
       <c r="E73" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>74</v>
       </c>
@@ -4452,8 +4674,11 @@
       <c r="E74" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4469,8 +4694,11 @@
       <c r="E75" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G75">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>58</v>
       </c>
@@ -4486,8 +4714,11 @@
       <c r="E76" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G76">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>58</v>
       </c>
@@ -4503,8 +4734,11 @@
       <c r="E77" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G77">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>58</v>
       </c>
@@ -4520,8 +4754,11 @@
       <c r="E78" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G78">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>97</v>
       </c>
@@ -4537,8 +4774,11 @@
       <c r="E79" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>97</v>
       </c>
@@ -4554,8 +4794,11 @@
       <c r="E80" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>90</v>
       </c>
@@ -4571,8 +4814,11 @@
       <c r="E81" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G81">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>90</v>
       </c>
@@ -4588,8 +4834,11 @@
       <c r="E82" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G82">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>70</v>
       </c>
@@ -4605,8 +4854,11 @@
       <c r="E83" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G83">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>70</v>
       </c>
@@ -4622,8 +4874,11 @@
       <c r="E84" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G84">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>70</v>
       </c>
@@ -4639,8 +4894,11 @@
       <c r="E85" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G85">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>41</v>
       </c>
@@ -4656,8 +4914,11 @@
       <c r="E86" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>41</v>
       </c>
@@ -4673,8 +4934,11 @@
       <c r="E87" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>28</v>
       </c>
@@ -4690,8 +4954,11 @@
       <c r="E88" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>28</v>
       </c>
@@ -4707,8 +4974,11 @@
       <c r="E89" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G89">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>22</v>
       </c>
@@ -4724,8 +4994,11 @@
       <c r="E90" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G90">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>22</v>
       </c>
@@ -4741,8 +5014,11 @@
       <c r="E91" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G91">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>22</v>
       </c>
@@ -4758,8 +5034,11 @@
       <c r="E92" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G92">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>47</v>
       </c>
@@ -4775,8 +5054,11 @@
       <c r="E93" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>47</v>
       </c>
@@ -4792,8 +5074,11 @@
       <c r="E94" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>34</v>
       </c>
@@ -4809,8 +5094,11 @@
       <c r="E95" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G95">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>34</v>
       </c>
@@ -4826,8 +5114,11 @@
       <c r="E96" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G96">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>27</v>
       </c>
@@ -4843,8 +5134,11 @@
       <c r="E97" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G97">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>27</v>
       </c>
@@ -4860,8 +5154,11 @@
       <c r="E98" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G98">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>27</v>
       </c>
@@ -4877,8 +5174,11 @@
       <c r="E99" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G99">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>55</v>
       </c>
@@ -4894,8 +5194,11 @@
       <c r="E100" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>55</v>
       </c>
@@ -4911,8 +5214,11 @@
       <c r="E101" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>41</v>
       </c>
@@ -4928,8 +5234,11 @@
       <c r="E102" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G102">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>41</v>
       </c>
@@ -4945,8 +5254,11 @@
       <c r="E103" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G103">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>32</v>
       </c>
@@ -4962,8 +5274,11 @@
       <c r="E104" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G104">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>32</v>
       </c>
@@ -4979,8 +5294,11 @@
       <c r="E105" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G105">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>32</v>
       </c>
@@ -4996,8 +5314,11 @@
       <c r="E106" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G106">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>63</v>
       </c>
@@ -5013,8 +5334,11 @@
       <c r="E107" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>63</v>
       </c>
@@ -5030,8 +5354,11 @@
       <c r="E108" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>50</v>
       </c>
@@ -5047,8 +5374,11 @@
       <c r="E109" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G109">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>50</v>
       </c>
@@ -5064,8 +5394,11 @@
       <c r="E110" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G110">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>39</v>
       </c>
@@ -5081,8 +5414,11 @@
       <c r="E111" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G111">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>39</v>
       </c>
@@ -5098,8 +5434,11 @@
       <c r="E112" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G112">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>39</v>
       </c>
@@ -5115,8 +5454,11 @@
       <c r="E113" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G113">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>73</v>
       </c>
@@ -5132,8 +5474,11 @@
       <c r="E114" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>73</v>
       </c>
@@ -5149,8 +5494,11 @@
       <c r="E115" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>61</v>
       </c>
@@ -5166,8 +5514,11 @@
       <c r="E116" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G116">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>61</v>
       </c>
@@ -5183,8 +5534,11 @@
       <c r="E117" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G117">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>47</v>
       </c>
@@ -5200,8 +5554,11 @@
       <c r="E118" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G118">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>47</v>
       </c>
@@ -5217,8 +5574,11 @@
       <c r="E119" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G119">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>47</v>
       </c>
@@ -5234,8 +5594,11 @@
       <c r="E120" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G120">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>73</v>
       </c>
@@ -5251,8 +5614,11 @@
       <c r="E121" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>73</v>
       </c>
@@ -5268,8 +5634,11 @@
       <c r="E122" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G122">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>61</v>
       </c>
@@ -5285,8 +5654,11 @@
       <c r="E123" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G123">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>61</v>
       </c>
@@ -5302,8 +5674,11 @@
       <c r="E124" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G124">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>47</v>
       </c>
@@ -5319,8 +5694,11 @@
       <c r="E125" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G125">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>47</v>
       </c>
@@ -5336,8 +5714,11 @@
       <c r="E126" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G126">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>47</v>
       </c>
@@ -5353,8 +5734,11 @@
       <c r="E127" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G127">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>84</v>
       </c>
@@ -5370,8 +5754,11 @@
       <c r="E128" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>84</v>
       </c>
@@ -5387,8 +5774,11 @@
       <c r="E129" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G129">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>74</v>
       </c>
@@ -5404,8 +5794,11 @@
       <c r="E130" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G130">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>74</v>
       </c>
@@ -5421,8 +5814,11 @@
       <c r="E131" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G131">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>58</v>
       </c>
@@ -5438,8 +5834,11 @@
       <c r="E132" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G132">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>58</v>
       </c>
@@ -5455,8 +5854,11 @@
       <c r="E133" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G133">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>58</v>
       </c>
@@ -5472,8 +5874,11 @@
       <c r="E134" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G134">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>97</v>
       </c>
@@ -5489,8 +5894,11 @@
       <c r="E135" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>97</v>
       </c>
@@ -5506,8 +5914,11 @@
       <c r="E136" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G136">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>90</v>
       </c>
@@ -5523,8 +5934,11 @@
       <c r="E137" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G137">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>90</v>
       </c>
@@ -5540,8 +5954,11 @@
       <c r="E138" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G138">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>70</v>
       </c>
@@ -5557,8 +5974,11 @@
       <c r="E139" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G139">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>70</v>
       </c>
@@ -5574,8 +5994,11 @@
       <c r="E140" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G140">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>70</v>
       </c>
@@ -5591,8 +6014,11 @@
       <c r="E141" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G141">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>112</v>
       </c>
@@ -5608,8 +6034,11 @@
       <c r="E142" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>112</v>
       </c>
@@ -5625,8 +6054,11 @@
       <c r="E143" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G143">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>109</v>
       </c>
@@ -5642,8 +6074,11 @@
       <c r="E144" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G144">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>109</v>
       </c>
@@ -5659,8 +6094,11 @@
       <c r="E145" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G145">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>85</v>
       </c>
@@ -5676,8 +6114,11 @@
       <c r="E146" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G146">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>85</v>
       </c>
@@ -5693,8 +6134,11 @@
       <c r="E147" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G147">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>85</v>
       </c>
@@ -5710,8 +6154,11 @@
       <c r="E148" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G148">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>112</v>
       </c>
@@ -5727,8 +6174,11 @@
       <c r="E149" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>112</v>
       </c>
@@ -5744,8 +6194,11 @@
       <c r="E150" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G150">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>109</v>
       </c>
@@ -5761,8 +6214,11 @@
       <c r="E151" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G151">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>109</v>
       </c>
@@ -5778,8 +6234,11 @@
       <c r="E152" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G152">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>85</v>
       </c>
@@ -5795,8 +6254,11 @@
       <c r="E153" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G153">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>85</v>
       </c>
@@ -5812,8 +6274,11 @@
       <c r="E154" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G154">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>85</v>
       </c>
@@ -5829,8 +6294,11 @@
       <c r="E155" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G155">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>128</v>
       </c>
@@ -5846,8 +6314,11 @@
       <c r="E156" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>128</v>
       </c>
@@ -5863,8 +6334,11 @@
       <c r="E157" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G157">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>133</v>
       </c>
@@ -5880,8 +6354,11 @@
       <c r="E158" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G158">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>133</v>
       </c>
@@ -5897,8 +6374,11 @@
       <c r="E159" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G159">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>102</v>
       </c>
@@ -5914,8 +6394,11 @@
       <c r="E160" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G160">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>102</v>
       </c>
@@ -5931,8 +6414,11 @@
       <c r="E161" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G161">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>102</v>
       </c>
@@ -5948,8 +6434,11 @@
       <c r="E162" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G162">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>147</v>
       </c>
@@ -5965,8 +6454,11 @@
       <c r="E163" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>147</v>
       </c>
@@ -5982,8 +6474,11 @@
       <c r="E164" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G164">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>161</v>
       </c>
@@ -5999,8 +6494,11 @@
       <c r="E165" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G165">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>161</v>
       </c>
@@ -6016,8 +6514,11 @@
       <c r="E166" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G166">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>124</v>
       </c>
@@ -6033,8 +6534,11 @@
       <c r="E167" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G167">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>124</v>
       </c>
@@ -6050,8 +6554,11 @@
       <c r="E168" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G168">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>124</v>
       </c>
@@ -6067,8 +6574,11 @@
       <c r="E169" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G169">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>182</v>
       </c>
@@ -6084,8 +6594,11 @@
       <c r="E170" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>182</v>
       </c>
@@ -6101,8 +6614,11 @@
       <c r="E171" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G171">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>212</v>
       </c>
@@ -6118,8 +6634,11 @@
       <c r="E172" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G172">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>212</v>
       </c>
@@ -6135,8 +6654,11 @@
       <c r="E173" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G173">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>162</v>
       </c>
@@ -6152,8 +6674,11 @@
       <c r="E174" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G174">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>162</v>
       </c>
@@ -6169,8 +6694,11 @@
       <c r="E175" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G175">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>162</v>
       </c>
@@ -6186,8 +6714,11 @@
       <c r="E176" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G176">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>128</v>
       </c>
@@ -6203,8 +6734,11 @@
       <c r="E177" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>128</v>
       </c>
@@ -6220,8 +6754,11 @@
       <c r="E178" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G178">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>133</v>
       </c>
@@ -6237,8 +6774,11 @@
       <c r="E179" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G179">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>133</v>
       </c>
@@ -6254,8 +6794,11 @@
       <c r="E180" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G180">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>102</v>
       </c>
@@ -6271,8 +6814,11 @@
       <c r="E181" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G181">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>102</v>
       </c>
@@ -6288,8 +6834,11 @@
       <c r="E182" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G182">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>102</v>
       </c>
@@ -6305,8 +6854,11 @@
       <c r="E183" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G183">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>147</v>
       </c>
@@ -6322,8 +6874,11 @@
       <c r="E184" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>147</v>
       </c>
@@ -6339,8 +6894,11 @@
       <c r="E185" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G185">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>161</v>
       </c>
@@ -6356,8 +6914,11 @@
       <c r="E186" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G186">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>161</v>
       </c>
@@ -6373,8 +6934,11 @@
       <c r="E187" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G187">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>124</v>
       </c>
@@ -6390,8 +6954,11 @@
       <c r="E188" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G188">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>124</v>
       </c>
@@ -6407,8 +6974,11 @@
       <c r="E189" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G189">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>124</v>
       </c>
@@ -6424,8 +6994,11 @@
       <c r="E190" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G190">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>182</v>
       </c>
@@ -6441,8 +7014,11 @@
       <c r="E191" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>182</v>
       </c>
@@ -6458,8 +7034,11 @@
       <c r="E192" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G192">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>212</v>
       </c>
@@ -6475,8 +7054,11 @@
       <c r="E193" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G193">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>212</v>
       </c>
@@ -6492,8 +7074,11 @@
       <c r="E194" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G194">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>162</v>
       </c>
@@ -6509,8 +7094,11 @@
       <c r="E195" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G195">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>162</v>
       </c>
@@ -6526,8 +7114,11 @@
       <c r="E196" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G196">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>162</v>
       </c>
@@ -6543,8 +7134,11 @@
       <c r="E197" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G197">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>224</v>
       </c>
@@ -6560,8 +7154,11 @@
       <c r="E198" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>224</v>
       </c>
@@ -6577,8 +7174,11 @@
       <c r="E199" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G199">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>277</v>
       </c>
@@ -6594,8 +7194,11 @@
       <c r="E200" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G200">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>277</v>
       </c>
@@ -6611,8 +7214,11 @@
       <c r="E201" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G201">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>212</v>
       </c>
@@ -6628,8 +7234,11 @@
       <c r="E202" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G202">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>212</v>
       </c>
@@ -6645,8 +7254,11 @@
       <c r="E203" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G203">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>212</v>
       </c>
@@ -6661,6 +7273,9 @@
       </c>
       <c r="E204" t="s">
         <v>81</v>
+      </c>
+      <c r="G204">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hide Criteria search and edit available
</commit_message>
<xml_diff>
--- a/test/xlsx/tablas_referencia.xlsx
+++ b/test/xlsx/tablas_referencia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorena/Documents/GitHub/rails_projects/rptconsultants/test/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5204FD5C-8039-4907-BD13-6709A2E33E51}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8021CB-97A9-3F47-855A-29B0E900CFD6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8835" activeTab="2" xr2:uid="{44D62DAF-BDC8-487B-86CE-15C7037211D0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="2" xr2:uid="{44D62DAF-BDC8-487B-86CE-15C7037211D0}"/>
   </bookViews>
   <sheets>
     <sheet name="grado" sheetId="1" r:id="rId1"/>
@@ -1816,65 +1816,65 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2196,9 +2196,9 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>18</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>3016</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="9">
         <v>17</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>2408</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>16</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>1807</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <v>15</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>1468</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>14</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>13</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>12</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>11</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <v>10</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="13">
         <v>8</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <v>7</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="13">
         <v>6</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <v>5</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="13">
         <v>4</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
         <v>3</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="13">
         <v>2</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>1</v>
       </c>
@@ -2477,12 +2477,12 @@
       <selection activeCell="D31" sqref="D31:E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21">
         <v>7</v>
       </c>
@@ -2506,12 +2506,12 @@
       <c r="C2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="106" t="s">
+      <c r="D2" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="107"/>
-    </row>
-    <row r="3" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="93"/>
+    </row>
+    <row r="3" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <v>6</v>
       </c>
@@ -2521,12 +2521,12 @@
       <c r="C3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="106" t="s">
+      <c r="D3" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="107"/>
-    </row>
-    <row r="4" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="93"/>
+    </row>
+    <row r="4" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <v>5</v>
       </c>
@@ -2536,12 +2536,12 @@
       <c r="C4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="106" t="s">
+      <c r="D4" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="107"/>
-    </row>
-    <row r="5" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="93"/>
+    </row>
+    <row r="5" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26">
         <v>4</v>
       </c>
@@ -2551,12 +2551,12 @@
       <c r="C5" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="106" t="s">
+      <c r="D5" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="107"/>
-    </row>
-    <row r="6" spans="1:5" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="93"/>
+    </row>
+    <row r="6" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29">
         <v>4</v>
       </c>
@@ -2566,12 +2566,12 @@
       <c r="C6" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="106" t="s">
+      <c r="D6" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="107"/>
-    </row>
-    <row r="7" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="93"/>
+    </row>
+    <row r="7" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26">
         <v>3</v>
       </c>
@@ -2581,12 +2581,12 @@
       <c r="C7" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="106" t="s">
+      <c r="D7" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="107"/>
-    </row>
-    <row r="8" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="93"/>
+    </row>
+    <row r="8" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31">
         <v>3</v>
       </c>
@@ -2596,12 +2596,12 @@
       <c r="C8" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="106" t="s">
+      <c r="D8" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="107"/>
-    </row>
-    <row r="9" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="93"/>
+    </row>
+    <row r="9" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
         <v>3</v>
       </c>
@@ -2611,12 +2611,12 @@
       <c r="C9" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="106" t="s">
+      <c r="D9" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="107"/>
-    </row>
-    <row r="10" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="93"/>
+    </row>
+    <row r="10" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <v>2</v>
       </c>
@@ -2626,12 +2626,12 @@
       <c r="C10" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="106" t="s">
+      <c r="D10" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="107"/>
-    </row>
-    <row r="11" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="93"/>
+    </row>
+    <row r="11" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
         <v>5</v>
       </c>
@@ -2641,38 +2641,38 @@
       <c r="C11" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="104" t="s">
+      <c r="D11" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="105"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="99"/>
+    </row>
+    <row r="12" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
         <v>4</v>
       </c>
-      <c r="B12" s="108" t="s">
+      <c r="B12" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="110" t="s">
+      <c r="C12" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="104" t="s">
+      <c r="D12" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="105"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="99"/>
+    </row>
+    <row r="13" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29">
         <v>4</v>
       </c>
-      <c r="B13" s="109"/>
-      <c r="C13" s="111"/>
-      <c r="D13" s="104" t="s">
+      <c r="B13" s="95"/>
+      <c r="C13" s="97"/>
+      <c r="D13" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="105"/>
-    </row>
-    <row r="14" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="99"/>
+    </row>
+    <row r="14" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
         <v>3</v>
       </c>
@@ -2682,23 +2682,23 @@
       <c r="C14" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="104" t="s">
+      <c r="D14" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="105"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="99"/>
+    </row>
+    <row r="15" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31">
         <v>3</v>
       </c>
       <c r="B15" s="37"/>
       <c r="C15" s="38"/>
-      <c r="D15" s="104" t="s">
+      <c r="D15" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="105"/>
-    </row>
-    <row r="16" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="99"/>
+    </row>
+    <row r="16" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
         <v>3</v>
       </c>
@@ -2708,12 +2708,12 @@
       <c r="C16" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="104" t="s">
+      <c r="D16" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="105"/>
-    </row>
-    <row r="17" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="99"/>
+    </row>
+    <row r="17" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21">
         <v>2</v>
       </c>
@@ -2723,12 +2723,12 @@
       <c r="C17" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="104" t="s">
+      <c r="D17" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="105"/>
-    </row>
-    <row r="18" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="99"/>
+    </row>
+    <row r="18" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="45">
         <v>1</v>
       </c>
@@ -2738,12 +2738,12 @@
       <c r="C18" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="104" t="s">
+      <c r="D18" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="105"/>
-    </row>
-    <row r="19" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="99"/>
+    </row>
+    <row r="19" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="45">
         <v>8</v>
       </c>
@@ -2753,12 +2753,12 @@
       <c r="C19" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="100" t="s">
+      <c r="D19" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="101"/>
-    </row>
-    <row r="20" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="103"/>
+    </row>
+    <row r="20" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21">
         <v>7</v>
       </c>
@@ -2768,12 +2768,12 @@
       <c r="C20" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="100" t="s">
+      <c r="D20" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="101"/>
-    </row>
-    <row r="21" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="103"/>
+    </row>
+    <row r="21" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21">
         <v>6</v>
       </c>
@@ -2783,12 +2783,12 @@
       <c r="C21" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="100" t="s">
+      <c r="D21" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="101"/>
-    </row>
-    <row r="22" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="103"/>
+    </row>
+    <row r="22" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21">
         <v>5</v>
       </c>
@@ -2798,12 +2798,12 @@
       <c r="C22" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="100" t="s">
+      <c r="D22" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="101"/>
-    </row>
-    <row r="23" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E22" s="103"/>
+    </row>
+    <row r="23" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21">
         <v>11</v>
       </c>
@@ -2813,12 +2813,12 @@
       <c r="C23" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="102" t="s">
+      <c r="D23" s="100" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="103"/>
-    </row>
-    <row r="24" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="101"/>
+    </row>
+    <row r="24" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21">
         <v>10</v>
       </c>
@@ -2828,12 +2828,12 @@
       <c r="C24" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="102" t="s">
+      <c r="D24" s="100" t="s">
         <v>51</v>
       </c>
-      <c r="E24" s="103"/>
-    </row>
-    <row r="25" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E24" s="101"/>
+    </row>
+    <row r="25" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="21">
         <v>9</v>
       </c>
@@ -2843,12 +2843,12 @@
       <c r="C25" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="102" t="s">
+      <c r="D25" s="100" t="s">
         <v>51</v>
       </c>
-      <c r="E25" s="103"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E25" s="101"/>
+    </row>
+    <row r="26" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21">
         <v>9</v>
       </c>
@@ -2858,12 +2858,12 @@
       <c r="C26" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="98" t="s">
+      <c r="D26" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="99"/>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E26" s="107"/>
+    </row>
+    <row r="27" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="45">
         <v>8</v>
       </c>
@@ -2873,12 +2873,12 @@
       <c r="C27" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="98" t="s">
+      <c r="D27" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="99"/>
-    </row>
-    <row r="28" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="107"/>
+    </row>
+    <row r="28" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="21">
         <v>7</v>
       </c>
@@ -2888,12 +2888,12 @@
       <c r="C28" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="D28" s="98" t="s">
+      <c r="D28" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="99"/>
-    </row>
-    <row r="29" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="107"/>
+    </row>
+    <row r="29" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="21">
         <v>6</v>
       </c>
@@ -2903,12 +2903,12 @@
       <c r="C29" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="98" t="s">
+      <c r="D29" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="99"/>
-    </row>
-    <row r="30" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="107"/>
+    </row>
+    <row r="30" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="21">
         <v>5</v>
       </c>
@@ -2918,12 +2918,12 @@
       <c r="C30" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="98" t="s">
+      <c r="D30" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="99"/>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E30" s="107"/>
+    </row>
+    <row r="31" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="31">
         <v>12</v>
       </c>
@@ -2933,12 +2933,12 @@
       <c r="C31" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="96" t="s">
+      <c r="D31" s="108" t="s">
         <v>66</v>
       </c>
-      <c r="E31" s="97"/>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E31" s="109"/>
+    </row>
+    <row r="32" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="21">
         <v>11</v>
       </c>
@@ -2948,12 +2948,12 @@
       <c r="C32" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="96" t="s">
+      <c r="D32" s="108" t="s">
         <v>66</v>
       </c>
-      <c r="E32" s="97"/>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E32" s="109"/>
+    </row>
+    <row r="33" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21">
         <v>10</v>
       </c>
@@ -2963,12 +2963,12 @@
       <c r="C33" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="96" t="s">
+      <c r="D33" s="108" t="s">
         <v>66</v>
       </c>
-      <c r="E33" s="97"/>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E33" s="109"/>
+    </row>
+    <row r="34" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21">
         <v>9</v>
       </c>
@@ -2978,12 +2978,12 @@
       <c r="C34" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="96" t="s">
+      <c r="D34" s="108" t="s">
         <v>66</v>
       </c>
-      <c r="E34" s="97"/>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E34" s="109"/>
+    </row>
+    <row r="35" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="21">
         <v>15</v>
       </c>
@@ -2993,12 +2993,12 @@
       <c r="C35" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="D35" s="94" t="s">
+      <c r="D35" s="104" t="s">
         <v>72</v>
       </c>
-      <c r="E35" s="95"/>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E35" s="105"/>
+    </row>
+    <row r="36" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="21">
         <v>14</v>
       </c>
@@ -3008,12 +3008,12 @@
       <c r="C36" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="94" t="s">
+      <c r="D36" s="104" t="s">
         <v>72</v>
       </c>
-      <c r="E36" s="95"/>
-    </row>
-    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E36" s="105"/>
+    </row>
+    <row r="37" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="73">
         <v>13</v>
       </c>
@@ -3023,12 +3023,12 @@
       <c r="C37" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="D37" s="94" t="s">
+      <c r="D37" s="104" t="s">
         <v>72</v>
       </c>
-      <c r="E37" s="95"/>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E37" s="105"/>
+    </row>
+    <row r="38" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="31">
         <v>12</v>
       </c>
@@ -3038,12 +3038,12 @@
       <c r="C38" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="D38" s="94" t="s">
+      <c r="D38" s="104" t="s">
         <v>72</v>
       </c>
-      <c r="E38" s="95"/>
-    </row>
-    <row r="39" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E38" s="105"/>
+    </row>
+    <row r="39" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="78">
         <v>18</v>
       </c>
@@ -3053,12 +3053,12 @@
       <c r="C39" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="D39" s="92" t="s">
+      <c r="D39" s="110" t="s">
         <v>81</v>
       </c>
-      <c r="E39" s="93"/>
-    </row>
-    <row r="40" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E39" s="111"/>
+    </row>
+    <row r="40" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="21">
         <v>17</v>
       </c>
@@ -3068,12 +3068,12 @@
       <c r="C40" s="77" t="s">
         <v>74</v>
       </c>
-      <c r="D40" s="92" t="s">
+      <c r="D40" s="110" t="s">
         <v>81</v>
       </c>
-      <c r="E40" s="93"/>
-    </row>
-    <row r="41" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E40" s="111"/>
+    </row>
+    <row r="41" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="21">
         <v>16</v>
       </c>
@@ -3083,12 +3083,12 @@
       <c r="C41" s="77" t="s">
         <v>74</v>
       </c>
-      <c r="D41" s="92" t="s">
+      <c r="D41" s="110" t="s">
         <v>81</v>
       </c>
-      <c r="E41" s="93"/>
-    </row>
-    <row r="42" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E41" s="111"/>
+    </row>
+    <row r="42" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="21">
         <v>15</v>
       </c>
@@ -3098,12 +3098,12 @@
       <c r="C42" s="77" t="s">
         <v>74</v>
       </c>
-      <c r="D42" s="92" t="s">
+      <c r="D42" s="110" t="s">
         <v>81</v>
       </c>
-      <c r="E42" s="93"/>
-    </row>
-    <row r="43" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E42" s="111"/>
+    </row>
+    <row r="43" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="21">
         <v>14</v>
       </c>
@@ -3113,12 +3113,12 @@
       <c r="C43" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="D43" s="92" t="s">
+      <c r="D43" s="110" t="s">
         <v>81</v>
       </c>
-      <c r="E43" s="93"/>
-    </row>
-    <row r="44" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E43" s="111"/>
+    </row>
+    <row r="44" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="73">
         <v>13</v>
       </c>
@@ -3128,27 +3128,32 @@
       <c r="C44" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="D44" s="92" t="s">
+      <c r="D44" s="110" t="s">
         <v>81</v>
       </c>
-      <c r="E44" s="93"/>
+      <c r="E44" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
@@ -3161,25 +3166,20 @@
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3187,18 +3187,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC65C15-1C40-4251-A583-2703229E8E4D}">
-  <dimension ref="A1:G204"/>
+  <dimension ref="A1:F204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="G191" sqref="G191:G204"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="37.83203125" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" customWidth="1"/>
     <col min="4" max="4" width="65" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>82</v>
       </c>
@@ -3214,11 +3218,11 @@
       <c r="E1" t="s">
         <v>100</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="164" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>23</v>
       </c>
@@ -3234,11 +3238,11 @@
       <c r="E2" t="s">
         <v>101</v>
       </c>
-      <c r="G2">
+      <c r="F2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="82" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>23</v>
       </c>
@@ -3254,11 +3258,11 @@
       <c r="E3" t="s">
         <v>101</v>
       </c>
-      <c r="G3">
+      <c r="F3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="115" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>13</v>
       </c>
@@ -3274,11 +3278,11 @@
       <c r="E4" t="s">
         <v>101</v>
       </c>
-      <c r="G4">
+      <c r="F4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="110.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="127" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>13</v>
       </c>
@@ -3294,11 +3298,11 @@
       <c r="E5" t="s">
         <v>101</v>
       </c>
-      <c r="G5">
+      <c r="F5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="104.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="107" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
@@ -3314,11 +3318,11 @@
       <c r="E6" t="s">
         <v>101</v>
       </c>
-      <c r="G6">
+      <c r="F6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="136.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="134" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10</v>
       </c>
@@ -3334,11 +3338,11 @@
       <c r="E7" t="s">
         <v>101</v>
       </c>
-      <c r="G7">
+      <c r="F7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="118.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="118" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10</v>
       </c>
@@ -3354,11 +3358,11 @@
       <c r="E8" t="s">
         <v>101</v>
       </c>
-      <c r="G8">
+      <c r="F8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="153.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="164" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>26</v>
       </c>
@@ -3374,11 +3378,11 @@
       <c r="E9" t="s">
         <v>101</v>
       </c>
-      <c r="G9">
+      <c r="F9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="82" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>26</v>
       </c>
@@ -3394,11 +3398,11 @@
       <c r="E10" t="s">
         <v>101</v>
       </c>
-      <c r="G10">
+      <c r="F10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="80.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="96" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>15</v>
       </c>
@@ -3414,11 +3418,11 @@
       <c r="E11" t="s">
         <v>101</v>
       </c>
-      <c r="G11">
+      <c r="F11">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="110.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="127" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>15</v>
       </c>
@@ -3434,11 +3438,11 @@
       <c r="E12" t="s">
         <v>101</v>
       </c>
-      <c r="G12">
+      <c r="F12">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="104.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="107" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3454,11 +3458,11 @@
       <c r="E13" t="s">
         <v>101</v>
       </c>
-      <c r="G13">
+      <c r="F13">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="136.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="134" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3474,11 +3478,11 @@
       <c r="E14" t="s">
         <v>101</v>
       </c>
-      <c r="G14">
+      <c r="F14">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="118.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="118" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -3494,11 +3498,11 @@
       <c r="E15" t="s">
         <v>101</v>
       </c>
-      <c r="G15">
+      <c r="F15">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="164" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>30</v>
       </c>
@@ -3514,11 +3518,11 @@
       <c r="E16" t="s">
         <v>101</v>
       </c>
-      <c r="G16">
+      <c r="F16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="82" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>30</v>
       </c>
@@ -3534,11 +3538,11 @@
       <c r="E17" t="s">
         <v>101</v>
       </c>
-      <c r="G17">
+      <c r="F17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="80.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="96" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>19</v>
       </c>
@@ -3554,11 +3558,11 @@
       <c r="E18" t="s">
         <v>101</v>
       </c>
-      <c r="G18">
+      <c r="F18">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="110.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="127" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
@@ -3574,11 +3578,11 @@
       <c r="E19" t="s">
         <v>101</v>
       </c>
-      <c r="G19">
+      <c r="F19">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="104.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="107" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>15</v>
       </c>
@@ -3594,11 +3598,11 @@
       <c r="E20" t="s">
         <v>101</v>
       </c>
-      <c r="G20">
+      <c r="F20">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="136.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="134" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>15</v>
       </c>
@@ -3614,11 +3618,11 @@
       <c r="E21" t="s">
         <v>101</v>
       </c>
-      <c r="G21">
+      <c r="F21">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="118.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="118" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>15</v>
       </c>
@@ -3634,11 +3638,11 @@
       <c r="E22" t="s">
         <v>101</v>
       </c>
-      <c r="G22">
+      <c r="F22">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="164" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>35</v>
       </c>
@@ -3654,11 +3658,11 @@
       <c r="E23" t="s">
         <v>101</v>
       </c>
-      <c r="G23">
+      <c r="F23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="82" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>35</v>
       </c>
@@ -3674,11 +3678,11 @@
       <c r="E24" t="s">
         <v>101</v>
       </c>
-      <c r="G24">
+      <c r="F24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="80.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="96" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3694,11 +3698,11 @@
       <c r="E25" t="s">
         <v>101</v>
       </c>
-      <c r="G25">
+      <c r="F25">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="110.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="127" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
@@ -3714,11 +3718,11 @@
       <c r="E26" t="s">
         <v>101</v>
       </c>
-      <c r="G26">
+      <c r="F26">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="104.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="107" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>18</v>
       </c>
@@ -3734,11 +3738,11 @@
       <c r="E27" t="s">
         <v>101</v>
       </c>
-      <c r="G27">
+      <c r="F27">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="136.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="134" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>18</v>
       </c>
@@ -3754,11 +3758,11 @@
       <c r="E28" t="s">
         <v>101</v>
       </c>
-      <c r="G28">
+      <c r="F28">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="118.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="118" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>18</v>
       </c>
@@ -3774,11 +3778,11 @@
       <c r="E29" t="s">
         <v>101</v>
       </c>
-      <c r="G29">
+      <c r="F29">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="164" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>41</v>
       </c>
@@ -3794,11 +3798,11 @@
       <c r="E30" t="s">
         <v>101</v>
       </c>
-      <c r="G30">
+      <c r="F30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="82" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>41</v>
       </c>
@@ -3814,11 +3818,11 @@
       <c r="E31" t="s">
         <v>101</v>
       </c>
-      <c r="G31">
+      <c r="F31">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="80.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="96" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>28</v>
       </c>
@@ -3834,11 +3838,11 @@
       <c r="E32" t="s">
         <v>101</v>
       </c>
-      <c r="G32">
+      <c r="F32">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="110.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="127" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>28</v>
       </c>
@@ -3854,11 +3858,11 @@
       <c r="E33" t="s">
         <v>101</v>
       </c>
-      <c r="G33">
+      <c r="F33">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="104.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="107" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>22</v>
       </c>
@@ -3874,11 +3878,11 @@
       <c r="E34" t="s">
         <v>101</v>
       </c>
-      <c r="G34">
+      <c r="F34">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="136.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="134" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>22</v>
       </c>
@@ -3894,11 +3898,11 @@
       <c r="E35" t="s">
         <v>101</v>
       </c>
-      <c r="G35">
+      <c r="F35">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="118.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="118" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>22</v>
       </c>
@@ -3914,11 +3918,11 @@
       <c r="E36" t="s">
         <v>101</v>
       </c>
-      <c r="G36">
+      <c r="F36">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>41</v>
       </c>
@@ -3934,11 +3938,11 @@
       <c r="E37" t="s">
         <v>128</v>
       </c>
-      <c r="G37">
+      <c r="F37">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>41</v>
       </c>
@@ -3954,11 +3958,11 @@
       <c r="E38" t="s">
         <v>128</v>
       </c>
-      <c r="G38">
+      <c r="F38">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>28</v>
       </c>
@@ -3974,11 +3978,11 @@
       <c r="E39" t="s">
         <v>128</v>
       </c>
-      <c r="G39">
+      <c r="F39">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>28</v>
       </c>
@@ -3994,11 +3998,11 @@
       <c r="E40" t="s">
         <v>128</v>
       </c>
-      <c r="G40">
+      <c r="F40">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>22</v>
       </c>
@@ -4014,11 +4018,11 @@
       <c r="E41" t="s">
         <v>128</v>
       </c>
-      <c r="G41">
+      <c r="F41">
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>22</v>
       </c>
@@ -4034,11 +4038,11 @@
       <c r="E42" t="s">
         <v>128</v>
       </c>
-      <c r="G42">
+      <c r="F42">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>22</v>
       </c>
@@ -4054,11 +4058,11 @@
       <c r="E43" t="s">
         <v>128</v>
       </c>
-      <c r="G43">
+      <c r="F43">
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>47</v>
       </c>
@@ -4074,11 +4078,11 @@
       <c r="E44" t="s">
         <v>128</v>
       </c>
-      <c r="G44">
+      <c r="F44">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>47</v>
       </c>
@@ -4094,11 +4098,11 @@
       <c r="E45" t="s">
         <v>128</v>
       </c>
-      <c r="G45">
+      <c r="F45">
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>34</v>
       </c>
@@ -4114,11 +4118,11 @@
       <c r="E46" t="s">
         <v>128</v>
       </c>
-      <c r="G46">
+      <c r="F46">
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>34</v>
       </c>
@@ -4134,11 +4138,11 @@
       <c r="E47" t="s">
         <v>128</v>
       </c>
-      <c r="G47">
+      <c r="F47">
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>27</v>
       </c>
@@ -4154,11 +4158,11 @@
       <c r="E48" t="s">
         <v>128</v>
       </c>
-      <c r="G48">
+      <c r="F48">
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>27</v>
       </c>
@@ -4174,11 +4178,11 @@
       <c r="E49" t="s">
         <v>128</v>
       </c>
-      <c r="G49">
+      <c r="F49">
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>27</v>
       </c>
@@ -4194,11 +4198,11 @@
       <c r="E50" t="s">
         <v>128</v>
       </c>
-      <c r="G50">
+      <c r="F50">
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>55</v>
       </c>
@@ -4214,11 +4218,11 @@
       <c r="E51" t="s">
         <v>128</v>
       </c>
-      <c r="G51">
+      <c r="F51">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>55</v>
       </c>
@@ -4234,11 +4238,11 @@
       <c r="E52" t="s">
         <v>128</v>
       </c>
-      <c r="G52">
+      <c r="F52">
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>41</v>
       </c>
@@ -4254,11 +4258,11 @@
       <c r="E53" t="s">
         <v>128</v>
       </c>
-      <c r="G53">
+      <c r="F53">
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>41</v>
       </c>
@@ -4274,11 +4278,11 @@
       <c r="E54" t="s">
         <v>128</v>
       </c>
-      <c r="G54">
+      <c r="F54">
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>32</v>
       </c>
@@ -4294,11 +4298,11 @@
       <c r="E55" t="s">
         <v>128</v>
       </c>
-      <c r="G55">
+      <c r="F55">
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>32</v>
       </c>
@@ -4314,11 +4318,11 @@
       <c r="E56" t="s">
         <v>128</v>
       </c>
-      <c r="G56">
+      <c r="F56">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>32</v>
       </c>
@@ -4334,11 +4338,11 @@
       <c r="E57" t="s">
         <v>128</v>
       </c>
-      <c r="G57">
+      <c r="F57">
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>63</v>
       </c>
@@ -4354,11 +4358,11 @@
       <c r="E58" t="s">
         <v>128</v>
       </c>
-      <c r="G58">
+      <c r="F58">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>63</v>
       </c>
@@ -4374,11 +4378,11 @@
       <c r="E59" t="s">
         <v>128</v>
       </c>
-      <c r="G59">
+      <c r="F59">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>50</v>
       </c>
@@ -4394,11 +4398,11 @@
       <c r="E60" t="s">
         <v>128</v>
       </c>
-      <c r="G60">
+      <c r="F60">
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>50</v>
       </c>
@@ -4414,11 +4418,11 @@
       <c r="E61" t="s">
         <v>128</v>
       </c>
-      <c r="G61">
+      <c r="F61">
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>39</v>
       </c>
@@ -4434,11 +4438,11 @@
       <c r="E62" t="s">
         <v>128</v>
       </c>
-      <c r="G62">
+      <c r="F62">
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>39</v>
       </c>
@@ -4454,11 +4458,11 @@
       <c r="E63" t="s">
         <v>128</v>
       </c>
-      <c r="G63">
+      <c r="F63">
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>39</v>
       </c>
@@ -4474,11 +4478,11 @@
       <c r="E64" t="s">
         <v>128</v>
       </c>
-      <c r="G64">
+      <c r="F64">
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>73</v>
       </c>
@@ -4494,11 +4498,11 @@
       <c r="E65" t="s">
         <v>157</v>
       </c>
-      <c r="G65">
+      <c r="F65">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>73</v>
       </c>
@@ -4514,11 +4518,11 @@
       <c r="E66" t="s">
         <v>157</v>
       </c>
-      <c r="G66">
+      <c r="F66">
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>61</v>
       </c>
@@ -4534,11 +4538,11 @@
       <c r="E67" t="s">
         <v>157</v>
       </c>
-      <c r="G67">
+      <c r="F67">
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>61</v>
       </c>
@@ -4554,11 +4558,11 @@
       <c r="E68" t="s">
         <v>157</v>
       </c>
-      <c r="G68">
+      <c r="F68">
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>47</v>
       </c>
@@ -4574,11 +4578,11 @@
       <c r="E69" t="s">
         <v>157</v>
       </c>
-      <c r="G69">
+      <c r="F69">
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>47</v>
       </c>
@@ -4594,11 +4598,11 @@
       <c r="E70" t="s">
         <v>157</v>
       </c>
-      <c r="G70">
+      <c r="F70">
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>47</v>
       </c>
@@ -4614,11 +4618,11 @@
       <c r="E71" t="s">
         <v>157</v>
       </c>
-      <c r="G71">
+      <c r="F71">
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>84</v>
       </c>
@@ -4634,11 +4638,11 @@
       <c r="E72" t="s">
         <v>157</v>
       </c>
-      <c r="G72">
+      <c r="F72">
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>84</v>
       </c>
@@ -4654,11 +4658,11 @@
       <c r="E73" t="s">
         <v>157</v>
       </c>
-      <c r="G73">
+      <c r="F73">
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>74</v>
       </c>
@@ -4674,11 +4678,11 @@
       <c r="E74" t="s">
         <v>157</v>
       </c>
-      <c r="G74">
+      <c r="F74">
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4694,11 +4698,11 @@
       <c r="E75" t="s">
         <v>157</v>
       </c>
-      <c r="G75">
+      <c r="F75">
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>58</v>
       </c>
@@ -4714,11 +4718,11 @@
       <c r="E76" t="s">
         <v>157</v>
       </c>
-      <c r="G76">
+      <c r="F76">
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>58</v>
       </c>
@@ -4734,11 +4738,11 @@
       <c r="E77" t="s">
         <v>157</v>
       </c>
-      <c r="G77">
+      <c r="F77">
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>58</v>
       </c>
@@ -4754,11 +4758,11 @@
       <c r="E78" t="s">
         <v>157</v>
       </c>
-      <c r="G78">
+      <c r="F78">
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>97</v>
       </c>
@@ -4774,11 +4778,11 @@
       <c r="E79" t="s">
         <v>157</v>
       </c>
-      <c r="G79">
+      <c r="F79">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>97</v>
       </c>
@@ -4794,11 +4798,11 @@
       <c r="E80" t="s">
         <v>157</v>
       </c>
-      <c r="G80">
+      <c r="F80">
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>90</v>
       </c>
@@ -4814,11 +4818,11 @@
       <c r="E81" t="s">
         <v>157</v>
       </c>
-      <c r="G81">
+      <c r="F81">
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>90</v>
       </c>
@@ -4834,11 +4838,11 @@
       <c r="E82" t="s">
         <v>157</v>
       </c>
-      <c r="G82">
+      <c r="F82">
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>70</v>
       </c>
@@ -4854,11 +4858,11 @@
       <c r="E83" t="s">
         <v>157</v>
       </c>
-      <c r="G83">
+      <c r="F83">
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>70</v>
       </c>
@@ -4874,11 +4878,11 @@
       <c r="E84" t="s">
         <v>157</v>
       </c>
-      <c r="G84">
+      <c r="F84">
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>70</v>
       </c>
@@ -4894,11 +4898,11 @@
       <c r="E85" t="s">
         <v>157</v>
       </c>
-      <c r="G85">
+      <c r="F85">
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>41</v>
       </c>
@@ -4914,11 +4918,11 @@
       <c r="E86" t="s">
         <v>176</v>
       </c>
-      <c r="G86">
+      <c r="F86">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>41</v>
       </c>
@@ -4934,11 +4938,11 @@
       <c r="E87" t="s">
         <v>176</v>
       </c>
-      <c r="G87">
+      <c r="F87">
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>28</v>
       </c>
@@ -4954,11 +4958,11 @@
       <c r="E88" t="s">
         <v>176</v>
       </c>
-      <c r="G88">
+      <c r="F88">
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>28</v>
       </c>
@@ -4974,11 +4978,11 @@
       <c r="E89" t="s">
         <v>176</v>
       </c>
-      <c r="G89">
+      <c r="F89">
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>22</v>
       </c>
@@ -4994,11 +4998,11 @@
       <c r="E90" t="s">
         <v>176</v>
       </c>
-      <c r="G90">
+      <c r="F90">
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>22</v>
       </c>
@@ -5014,11 +5018,11 @@
       <c r="E91" t="s">
         <v>176</v>
       </c>
-      <c r="G91">
+      <c r="F91">
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>22</v>
       </c>
@@ -5034,11 +5038,11 @@
       <c r="E92" t="s">
         <v>176</v>
       </c>
-      <c r="G92">
+      <c r="F92">
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>47</v>
       </c>
@@ -5054,11 +5058,11 @@
       <c r="E93" t="s">
         <v>176</v>
       </c>
-      <c r="G93">
+      <c r="F93">
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>47</v>
       </c>
@@ -5074,11 +5078,11 @@
       <c r="E94" t="s">
         <v>176</v>
       </c>
-      <c r="G94">
+      <c r="F94">
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>34</v>
       </c>
@@ -5094,11 +5098,11 @@
       <c r="E95" t="s">
         <v>176</v>
       </c>
-      <c r="G95">
+      <c r="F95">
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>34</v>
       </c>
@@ -5114,11 +5118,11 @@
       <c r="E96" t="s">
         <v>176</v>
       </c>
-      <c r="G96">
+      <c r="F96">
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>27</v>
       </c>
@@ -5134,11 +5138,11 @@
       <c r="E97" t="s">
         <v>176</v>
       </c>
-      <c r="G97">
+      <c r="F97">
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>27</v>
       </c>
@@ -5154,11 +5158,11 @@
       <c r="E98" t="s">
         <v>176</v>
       </c>
-      <c r="G98">
+      <c r="F98">
         <v>6</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>27</v>
       </c>
@@ -5174,11 +5178,11 @@
       <c r="E99" t="s">
         <v>176</v>
       </c>
-      <c r="G99">
+      <c r="F99">
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>55</v>
       </c>
@@ -5194,11 +5198,11 @@
       <c r="E100" t="s">
         <v>176</v>
       </c>
-      <c r="G100">
+      <c r="F100">
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>55</v>
       </c>
@@ -5214,11 +5218,11 @@
       <c r="E101" t="s">
         <v>176</v>
       </c>
-      <c r="G101">
+      <c r="F101">
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>41</v>
       </c>
@@ -5234,11 +5238,11 @@
       <c r="E102" t="s">
         <v>176</v>
       </c>
-      <c r="G102">
+      <c r="F102">
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>41</v>
       </c>
@@ -5254,11 +5258,11 @@
       <c r="E103" t="s">
         <v>176</v>
       </c>
-      <c r="G103">
+      <c r="F103">
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>32</v>
       </c>
@@ -5274,11 +5278,11 @@
       <c r="E104" t="s">
         <v>176</v>
       </c>
-      <c r="G104">
+      <c r="F104">
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>32</v>
       </c>
@@ -5294,11 +5298,11 @@
       <c r="E105" t="s">
         <v>176</v>
       </c>
-      <c r="G105">
+      <c r="F105">
         <v>6</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>32</v>
       </c>
@@ -5314,11 +5318,11 @@
       <c r="E106" t="s">
         <v>176</v>
       </c>
-      <c r="G106">
+      <c r="F106">
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>63</v>
       </c>
@@ -5334,11 +5338,11 @@
       <c r="E107" t="s">
         <v>176</v>
       </c>
-      <c r="G107">
+      <c r="F107">
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>63</v>
       </c>
@@ -5354,11 +5358,11 @@
       <c r="E108" t="s">
         <v>176</v>
       </c>
-      <c r="G108">
+      <c r="F108">
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>50</v>
       </c>
@@ -5374,11 +5378,11 @@
       <c r="E109" t="s">
         <v>176</v>
       </c>
-      <c r="G109">
+      <c r="F109">
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>50</v>
       </c>
@@ -5394,11 +5398,11 @@
       <c r="E110" t="s">
         <v>176</v>
       </c>
-      <c r="G110">
+      <c r="F110">
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>39</v>
       </c>
@@ -5414,11 +5418,11 @@
       <c r="E111" t="s">
         <v>176</v>
       </c>
-      <c r="G111">
+      <c r="F111">
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>39</v>
       </c>
@@ -5434,11 +5438,11 @@
       <c r="E112" t="s">
         <v>176</v>
       </c>
-      <c r="G112">
+      <c r="F112">
         <v>6</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>39</v>
       </c>
@@ -5454,11 +5458,11 @@
       <c r="E113" t="s">
         <v>176</v>
       </c>
-      <c r="G113">
+      <c r="F113">
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>73</v>
       </c>
@@ -5474,11 +5478,11 @@
       <c r="E114" t="s">
         <v>176</v>
       </c>
-      <c r="G114">
+      <c r="F114">
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>73</v>
       </c>
@@ -5494,11 +5498,11 @@
       <c r="E115" t="s">
         <v>176</v>
       </c>
-      <c r="G115">
+      <c r="F115">
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>61</v>
       </c>
@@ -5514,11 +5518,11 @@
       <c r="E116" t="s">
         <v>176</v>
       </c>
-      <c r="G116">
+      <c r="F116">
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>61</v>
       </c>
@@ -5534,11 +5538,11 @@
       <c r="E117" t="s">
         <v>176</v>
       </c>
-      <c r="G117">
+      <c r="F117">
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>47</v>
       </c>
@@ -5554,11 +5558,11 @@
       <c r="E118" t="s">
         <v>176</v>
       </c>
-      <c r="G118">
+      <c r="F118">
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>47</v>
       </c>
@@ -5574,11 +5578,11 @@
       <c r="E119" t="s">
         <v>176</v>
       </c>
-      <c r="G119">
+      <c r="F119">
         <v>6</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>47</v>
       </c>
@@ -5594,11 +5598,11 @@
       <c r="E120" t="s">
         <v>176</v>
       </c>
-      <c r="G120">
+      <c r="F120">
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>73</v>
       </c>
@@ -5614,11 +5618,11 @@
       <c r="E121" t="s">
         <v>206</v>
       </c>
-      <c r="G121">
+      <c r="F121">
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>73</v>
       </c>
@@ -5634,11 +5638,11 @@
       <c r="E122" t="s">
         <v>206</v>
       </c>
-      <c r="G122">
+      <c r="F122">
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>61</v>
       </c>
@@ -5654,11 +5658,11 @@
       <c r="E123" t="s">
         <v>206</v>
       </c>
-      <c r="G123">
+      <c r="F123">
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>61</v>
       </c>
@@ -5674,11 +5678,11 @@
       <c r="E124" t="s">
         <v>206</v>
       </c>
-      <c r="G124">
+      <c r="F124">
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>47</v>
       </c>
@@ -5694,11 +5698,11 @@
       <c r="E125" t="s">
         <v>206</v>
       </c>
-      <c r="G125">
+      <c r="F125">
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>47</v>
       </c>
@@ -5714,11 +5718,11 @@
       <c r="E126" t="s">
         <v>206</v>
       </c>
-      <c r="G126">
+      <c r="F126">
         <v>6</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>47</v>
       </c>
@@ -5734,11 +5738,11 @@
       <c r="E127" t="s">
         <v>206</v>
       </c>
-      <c r="G127">
+      <c r="F127">
         <v>7</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>84</v>
       </c>
@@ -5754,11 +5758,11 @@
       <c r="E128" t="s">
         <v>206</v>
       </c>
-      <c r="G128">
+      <c r="F128">
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>84</v>
       </c>
@@ -5774,11 +5778,11 @@
       <c r="E129" t="s">
         <v>206</v>
       </c>
-      <c r="G129">
+      <c r="F129">
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>74</v>
       </c>
@@ -5794,11 +5798,11 @@
       <c r="E130" t="s">
         <v>206</v>
       </c>
-      <c r="G130">
+      <c r="F130">
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>74</v>
       </c>
@@ -5814,11 +5818,11 @@
       <c r="E131" t="s">
         <v>206</v>
       </c>
-      <c r="G131">
+      <c r="F131">
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>58</v>
       </c>
@@ -5834,11 +5838,11 @@
       <c r="E132" t="s">
         <v>206</v>
       </c>
-      <c r="G132">
+      <c r="F132">
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>58</v>
       </c>
@@ -5854,11 +5858,11 @@
       <c r="E133" t="s">
         <v>206</v>
       </c>
-      <c r="G133">
+      <c r="F133">
         <v>6</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>58</v>
       </c>
@@ -5874,11 +5878,11 @@
       <c r="E134" t="s">
         <v>206</v>
       </c>
-      <c r="G134">
+      <c r="F134">
         <v>7</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>97</v>
       </c>
@@ -5894,11 +5898,11 @@
       <c r="E135" t="s">
         <v>206</v>
       </c>
-      <c r="G135">
+      <c r="F135">
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>97</v>
       </c>
@@ -5914,11 +5918,11 @@
       <c r="E136" t="s">
         <v>206</v>
       </c>
-      <c r="G136">
+      <c r="F136">
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>90</v>
       </c>
@@ -5934,11 +5938,11 @@
       <c r="E137" t="s">
         <v>206</v>
       </c>
-      <c r="G137">
+      <c r="F137">
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>90</v>
       </c>
@@ -5954,11 +5958,11 @@
       <c r="E138" t="s">
         <v>206</v>
       </c>
-      <c r="G138">
+      <c r="F138">
         <v>4</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>70</v>
       </c>
@@ -5974,11 +5978,11 @@
       <c r="E139" t="s">
         <v>206</v>
       </c>
-      <c r="G139">
+      <c r="F139">
         <v>5</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>70</v>
       </c>
@@ -5994,11 +5998,11 @@
       <c r="E140" t="s">
         <v>206</v>
       </c>
-      <c r="G140">
+      <c r="F140">
         <v>6</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>70</v>
       </c>
@@ -6014,11 +6018,11 @@
       <c r="E141" t="s">
         <v>206</v>
       </c>
-      <c r="G141">
+      <c r="F141">
         <v>7</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>112</v>
       </c>
@@ -6034,11 +6038,11 @@
       <c r="E142" t="s">
         <v>206</v>
       </c>
-      <c r="G142">
+      <c r="F142">
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>112</v>
       </c>
@@ -6054,11 +6058,11 @@
       <c r="E143" t="s">
         <v>206</v>
       </c>
-      <c r="G143">
+      <c r="F143">
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>109</v>
       </c>
@@ -6074,11 +6078,11 @@
       <c r="E144" t="s">
         <v>206</v>
       </c>
-      <c r="G144">
+      <c r="F144">
         <v>3</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>109</v>
       </c>
@@ -6094,11 +6098,11 @@
       <c r="E145" t="s">
         <v>206</v>
       </c>
-      <c r="G145">
+      <c r="F145">
         <v>4</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>85</v>
       </c>
@@ -6114,11 +6118,11 @@
       <c r="E146" t="s">
         <v>206</v>
       </c>
-      <c r="G146">
+      <c r="F146">
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>85</v>
       </c>
@@ -6134,11 +6138,11 @@
       <c r="E147" t="s">
         <v>206</v>
       </c>
-      <c r="G147">
+      <c r="F147">
         <v>6</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>85</v>
       </c>
@@ -6154,11 +6158,11 @@
       <c r="E148" t="s">
         <v>206</v>
       </c>
-      <c r="G148">
+      <c r="F148">
         <v>7</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>112</v>
       </c>
@@ -6174,11 +6178,11 @@
       <c r="E149" t="s">
         <v>228</v>
       </c>
-      <c r="G149">
+      <c r="F149">
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>112</v>
       </c>
@@ -6194,11 +6198,11 @@
       <c r="E150" t="s">
         <v>228</v>
       </c>
-      <c r="G150">
+      <c r="F150">
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>109</v>
       </c>
@@ -6214,11 +6218,11 @@
       <c r="E151" t="s">
         <v>228</v>
       </c>
-      <c r="G151">
+      <c r="F151">
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>109</v>
       </c>
@@ -6234,11 +6238,11 @@
       <c r="E152" t="s">
         <v>228</v>
       </c>
-      <c r="G152">
+      <c r="F152">
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>85</v>
       </c>
@@ -6254,11 +6258,11 @@
       <c r="E153" t="s">
         <v>228</v>
       </c>
-      <c r="G153">
+      <c r="F153">
         <v>5</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>85</v>
       </c>
@@ -6274,11 +6278,11 @@
       <c r="E154" t="s">
         <v>228</v>
       </c>
-      <c r="G154">
+      <c r="F154">
         <v>6</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>85</v>
       </c>
@@ -6294,11 +6298,11 @@
       <c r="E155" t="s">
         <v>228</v>
       </c>
-      <c r="G155">
+      <c r="F155">
         <v>7</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>128</v>
       </c>
@@ -6314,11 +6318,11 @@
       <c r="E156" t="s">
         <v>228</v>
       </c>
-      <c r="G156">
+      <c r="F156">
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>128</v>
       </c>
@@ -6334,11 +6338,11 @@
       <c r="E157" t="s">
         <v>228</v>
       </c>
-      <c r="G157">
+      <c r="F157">
         <v>2</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>133</v>
       </c>
@@ -6354,11 +6358,11 @@
       <c r="E158" t="s">
         <v>228</v>
       </c>
-      <c r="G158">
+      <c r="F158">
         <v>3</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>133</v>
       </c>
@@ -6374,11 +6378,11 @@
       <c r="E159" t="s">
         <v>228</v>
       </c>
-      <c r="G159">
+      <c r="F159">
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>102</v>
       </c>
@@ -6394,11 +6398,11 @@
       <c r="E160" t="s">
         <v>228</v>
       </c>
-      <c r="G160">
+      <c r="F160">
         <v>5</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>102</v>
       </c>
@@ -6414,11 +6418,11 @@
       <c r="E161" t="s">
         <v>228</v>
       </c>
-      <c r="G161">
+      <c r="F161">
         <v>6</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>102</v>
       </c>
@@ -6434,11 +6438,11 @@
       <c r="E162" t="s">
         <v>228</v>
       </c>
-      <c r="G162">
+      <c r="F162">
         <v>7</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>147</v>
       </c>
@@ -6454,11 +6458,11 @@
       <c r="E163" t="s">
         <v>228</v>
       </c>
-      <c r="G163">
+      <c r="F163">
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>147</v>
       </c>
@@ -6474,11 +6478,11 @@
       <c r="E164" t="s">
         <v>228</v>
       </c>
-      <c r="G164">
+      <c r="F164">
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>161</v>
       </c>
@@ -6494,11 +6498,11 @@
       <c r="E165" t="s">
         <v>228</v>
       </c>
-      <c r="G165">
+      <c r="F165">
         <v>3</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>161</v>
       </c>
@@ -6514,11 +6518,11 @@
       <c r="E166" t="s">
         <v>228</v>
       </c>
-      <c r="G166">
+      <c r="F166">
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>124</v>
       </c>
@@ -6534,11 +6538,11 @@
       <c r="E167" t="s">
         <v>228</v>
       </c>
-      <c r="G167">
+      <c r="F167">
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>124</v>
       </c>
@@ -6554,11 +6558,11 @@
       <c r="E168" t="s">
         <v>228</v>
       </c>
-      <c r="G168">
+      <c r="F168">
         <v>6</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>124</v>
       </c>
@@ -6574,11 +6578,11 @@
       <c r="E169" t="s">
         <v>228</v>
       </c>
-      <c r="G169">
+      <c r="F169">
         <v>7</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>182</v>
       </c>
@@ -6594,11 +6598,11 @@
       <c r="E170" t="s">
         <v>228</v>
       </c>
-      <c r="G170">
+      <c r="F170">
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>182</v>
       </c>
@@ -6614,11 +6618,11 @@
       <c r="E171" t="s">
         <v>228</v>
       </c>
-      <c r="G171">
+      <c r="F171">
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>212</v>
       </c>
@@ -6634,11 +6638,11 @@
       <c r="E172" t="s">
         <v>228</v>
       </c>
-      <c r="G172">
+      <c r="F172">
         <v>3</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>212</v>
       </c>
@@ -6654,11 +6658,11 @@
       <c r="E173" t="s">
         <v>228</v>
       </c>
-      <c r="G173">
+      <c r="F173">
         <v>4</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>162</v>
       </c>
@@ -6674,11 +6678,11 @@
       <c r="E174" t="s">
         <v>228</v>
       </c>
-      <c r="G174">
+      <c r="F174">
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>162</v>
       </c>
@@ -6694,11 +6698,11 @@
       <c r="E175" t="s">
         <v>228</v>
       </c>
-      <c r="G175">
+      <c r="F175">
         <v>6</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>162</v>
       </c>
@@ -6714,11 +6718,11 @@
       <c r="E176" t="s">
         <v>228</v>
       </c>
-      <c r="G176">
+      <c r="F176">
         <v>7</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>128</v>
       </c>
@@ -6734,11 +6738,11 @@
       <c r="E177" t="s">
         <v>81</v>
       </c>
-      <c r="G177">
+      <c r="F177">
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>128</v>
       </c>
@@ -6754,11 +6758,11 @@
       <c r="E178" t="s">
         <v>81</v>
       </c>
-      <c r="G178">
+      <c r="F178">
         <v>2</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>133</v>
       </c>
@@ -6774,11 +6778,11 @@
       <c r="E179" t="s">
         <v>81</v>
       </c>
-      <c r="G179">
+      <c r="F179">
         <v>3</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>133</v>
       </c>
@@ -6794,11 +6798,11 @@
       <c r="E180" t="s">
         <v>81</v>
       </c>
-      <c r="G180">
+      <c r="F180">
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>102</v>
       </c>
@@ -6814,11 +6818,11 @@
       <c r="E181" t="s">
         <v>81</v>
       </c>
-      <c r="G181">
+      <c r="F181">
         <v>5</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>102</v>
       </c>
@@ -6834,11 +6838,11 @@
       <c r="E182" t="s">
         <v>81</v>
       </c>
-      <c r="G182">
+      <c r="F182">
         <v>6</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>102</v>
       </c>
@@ -6854,11 +6858,11 @@
       <c r="E183" t="s">
         <v>81</v>
       </c>
-      <c r="G183">
+      <c r="F183">
         <v>7</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>147</v>
       </c>
@@ -6874,11 +6878,11 @@
       <c r="E184" t="s">
         <v>81</v>
       </c>
-      <c r="G184">
+      <c r="F184">
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>147</v>
       </c>
@@ -6894,11 +6898,11 @@
       <c r="E185" t="s">
         <v>81</v>
       </c>
-      <c r="G185">
+      <c r="F185">
         <v>2</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>161</v>
       </c>
@@ -6914,11 +6918,11 @@
       <c r="E186" t="s">
         <v>81</v>
       </c>
-      <c r="G186">
+      <c r="F186">
         <v>3</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>161</v>
       </c>
@@ -6934,11 +6938,11 @@
       <c r="E187" t="s">
         <v>81</v>
       </c>
-      <c r="G187">
+      <c r="F187">
         <v>4</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>124</v>
       </c>
@@ -6954,11 +6958,11 @@
       <c r="E188" t="s">
         <v>81</v>
       </c>
-      <c r="G188">
+      <c r="F188">
         <v>5</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>124</v>
       </c>
@@ -6974,11 +6978,11 @@
       <c r="E189" t="s">
         <v>81</v>
       </c>
-      <c r="G189">
+      <c r="F189">
         <v>6</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>124</v>
       </c>
@@ -6994,11 +6998,11 @@
       <c r="E190" t="s">
         <v>81</v>
       </c>
-      <c r="G190">
+      <c r="F190">
         <v>7</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>182</v>
       </c>
@@ -7014,11 +7018,11 @@
       <c r="E191" t="s">
         <v>81</v>
       </c>
-      <c r="G191">
+      <c r="F191">
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>182</v>
       </c>
@@ -7034,11 +7038,11 @@
       <c r="E192" t="s">
         <v>81</v>
       </c>
-      <c r="G192">
+      <c r="F192">
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>212</v>
       </c>
@@ -7054,11 +7058,11 @@
       <c r="E193" t="s">
         <v>81</v>
       </c>
-      <c r="G193">
+      <c r="F193">
         <v>3</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>212</v>
       </c>
@@ -7074,11 +7078,11 @@
       <c r="E194" t="s">
         <v>81</v>
       </c>
-      <c r="G194">
+      <c r="F194">
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>162</v>
       </c>
@@ -7094,11 +7098,11 @@
       <c r="E195" t="s">
         <v>81</v>
       </c>
-      <c r="G195">
+      <c r="F195">
         <v>5</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>162</v>
       </c>
@@ -7114,11 +7118,11 @@
       <c r="E196" t="s">
         <v>81</v>
       </c>
-      <c r="G196">
+      <c r="F196">
         <v>6</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>162</v>
       </c>
@@ -7134,11 +7138,11 @@
       <c r="E197" t="s">
         <v>81</v>
       </c>
-      <c r="G197">
+      <c r="F197">
         <v>7</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>224</v>
       </c>
@@ -7154,11 +7158,11 @@
       <c r="E198" t="s">
         <v>81</v>
       </c>
-      <c r="G198">
+      <c r="F198">
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>224</v>
       </c>
@@ -7174,11 +7178,11 @@
       <c r="E199" t="s">
         <v>81</v>
       </c>
-      <c r="G199">
+      <c r="F199">
         <v>2</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>277</v>
       </c>
@@ -7194,11 +7198,11 @@
       <c r="E200" t="s">
         <v>81</v>
       </c>
-      <c r="G200">
+      <c r="F200">
         <v>3</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>277</v>
       </c>
@@ -7214,11 +7218,11 @@
       <c r="E201" t="s">
         <v>81</v>
       </c>
-      <c r="G201">
+      <c r="F201">
         <v>4</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>212</v>
       </c>
@@ -7234,11 +7238,11 @@
       <c r="E202" t="s">
         <v>81</v>
       </c>
-      <c r="G202">
+      <c r="F202">
         <v>5</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>212</v>
       </c>
@@ -7254,11 +7258,11 @@
       <c r="E203" t="s">
         <v>81</v>
       </c>
-      <c r="G203">
+      <c r="F203">
         <v>6</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>212</v>
       </c>
@@ -7274,7 +7278,7 @@
       <c r="E204" t="s">
         <v>81</v>
       </c>
-      <c r="G204">
+      <c r="F204">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Edit available on criteria
</commit_message>
<xml_diff>
--- a/test/xlsx/tablas_referencia.xlsx
+++ b/test/xlsx/tablas_referencia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorena/Documents/GitHub/rails_projects/rptconsultants/test/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8021CB-97A9-3F47-855A-29B0E900CFD6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF774D5-BCB1-9444-9AAF-8C81DD5C73B0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="2" xr2:uid="{44D62DAF-BDC8-487B-86CE-15C7037211D0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{44D62DAF-BDC8-487B-86CE-15C7037211D0}"/>
   </bookViews>
   <sheets>
     <sheet name="grado" sheetId="1" r:id="rId1"/>
@@ -1816,6 +1816,48 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1833,48 +1875,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2473,13 +2473,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575881AF-8C00-4C5E-94D1-79C6F03A8C05}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31:E31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2506,10 +2506,10 @@
       <c r="C2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="92" t="s">
+      <c r="D2" s="106" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="93"/>
+      <c r="E2" s="107"/>
     </row>
     <row r="3" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
@@ -2521,10 +2521,10 @@
       <c r="C3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="92" t="s">
+      <c r="D3" s="106" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="93"/>
+      <c r="E3" s="107"/>
     </row>
     <row r="4" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
@@ -2536,10 +2536,10 @@
       <c r="C4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="92" t="s">
+      <c r="D4" s="106" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="93"/>
+      <c r="E4" s="107"/>
     </row>
     <row r="5" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26">
@@ -2551,10 +2551,10 @@
       <c r="C5" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="92" t="s">
+      <c r="D5" s="106" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="93"/>
+      <c r="E5" s="107"/>
     </row>
     <row r="6" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29">
@@ -2566,10 +2566,10 @@
       <c r="C6" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="92" t="s">
+      <c r="D6" s="106" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="93"/>
+      <c r="E6" s="107"/>
     </row>
     <row r="7" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26">
@@ -2581,10 +2581,10 @@
       <c r="C7" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="92" t="s">
+      <c r="D7" s="106" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="93"/>
+      <c r="E7" s="107"/>
     </row>
     <row r="8" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31">
@@ -2596,10 +2596,10 @@
       <c r="C8" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="92" t="s">
+      <c r="D8" s="106" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="93"/>
+      <c r="E8" s="107"/>
     </row>
     <row r="9" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
@@ -2611,10 +2611,10 @@
       <c r="C9" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="92" t="s">
+      <c r="D9" s="106" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="93"/>
+      <c r="E9" s="107"/>
     </row>
     <row r="10" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
@@ -2626,10 +2626,10 @@
       <c r="C10" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="92" t="s">
+      <c r="D10" s="106" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="93"/>
+      <c r="E10" s="107"/>
     </row>
     <row r="11" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
@@ -2641,36 +2641,36 @@
       <c r="C11" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="98" t="s">
+      <c r="D11" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="99"/>
+      <c r="E11" s="103"/>
     </row>
     <row r="12" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
         <v>4</v>
       </c>
-      <c r="B12" s="94" t="s">
+      <c r="B12" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="96" t="s">
+      <c r="C12" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="98" t="s">
+      <c r="D12" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="99"/>
+      <c r="E12" s="103"/>
     </row>
     <row r="13" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29">
         <v>4</v>
       </c>
-      <c r="B13" s="95"/>
-      <c r="C13" s="97"/>
-      <c r="D13" s="98" t="s">
+      <c r="B13" s="109"/>
+      <c r="C13" s="111"/>
+      <c r="D13" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="99"/>
+      <c r="E13" s="103"/>
     </row>
     <row r="14" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
@@ -2682,10 +2682,10 @@
       <c r="C14" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="98" t="s">
+      <c r="D14" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="99"/>
+      <c r="E14" s="103"/>
     </row>
     <row r="15" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31">
@@ -2693,10 +2693,10 @@
       </c>
       <c r="B15" s="37"/>
       <c r="C15" s="38"/>
-      <c r="D15" s="98" t="s">
+      <c r="D15" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="99"/>
+      <c r="E15" s="103"/>
     </row>
     <row r="16" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
@@ -2708,10 +2708,10 @@
       <c r="C16" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="98" t="s">
+      <c r="D16" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="99"/>
+      <c r="E16" s="103"/>
     </row>
     <row r="17" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21">
@@ -2723,10 +2723,10 @@
       <c r="C17" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="98" t="s">
+      <c r="D17" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="99"/>
+      <c r="E17" s="103"/>
     </row>
     <row r="18" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="45">
@@ -2738,10 +2738,10 @@
       <c r="C18" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="98" t="s">
+      <c r="D18" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="99"/>
+      <c r="E18" s="103"/>
     </row>
     <row r="19" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="45">
@@ -2753,10 +2753,10 @@
       <c r="C19" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="102" t="s">
+      <c r="D19" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="103"/>
+      <c r="E19" s="105"/>
     </row>
     <row r="20" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21">
@@ -2768,10 +2768,10 @@
       <c r="C20" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="102" t="s">
+      <c r="D20" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="103"/>
+      <c r="E20" s="105"/>
     </row>
     <row r="21" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21">
@@ -2783,10 +2783,10 @@
       <c r="C21" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="102" t="s">
+      <c r="D21" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="103"/>
+      <c r="E21" s="105"/>
     </row>
     <row r="22" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21">
@@ -2798,10 +2798,10 @@
       <c r="C22" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="102" t="s">
+      <c r="D22" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="103"/>
+      <c r="E22" s="105"/>
     </row>
     <row r="23" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21">
@@ -2858,10 +2858,10 @@
       <c r="C26" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="106" t="s">
+      <c r="D26" s="96" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="107"/>
+      <c r="E26" s="97"/>
     </row>
     <row r="27" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="45">
@@ -2873,10 +2873,10 @@
       <c r="C27" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="106" t="s">
+      <c r="D27" s="96" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="107"/>
+      <c r="E27" s="97"/>
     </row>
     <row r="28" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="21">
@@ -2888,10 +2888,10 @@
       <c r="C28" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="D28" s="106" t="s">
+      <c r="D28" s="96" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="107"/>
+      <c r="E28" s="97"/>
     </row>
     <row r="29" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="21">
@@ -2903,10 +2903,10 @@
       <c r="C29" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="106" t="s">
+      <c r="D29" s="96" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="107"/>
+      <c r="E29" s="97"/>
     </row>
     <row r="30" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="21">
@@ -2918,10 +2918,10 @@
       <c r="C30" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="106" t="s">
+      <c r="D30" s="96" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="107"/>
+      <c r="E30" s="97"/>
     </row>
     <row r="31" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="31">
@@ -2933,10 +2933,10 @@
       <c r="C31" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="108" t="s">
+      <c r="D31" s="98" t="s">
         <v>66</v>
       </c>
-      <c r="E31" s="109"/>
+      <c r="E31" s="99"/>
     </row>
     <row r="32" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="21">
@@ -2948,10 +2948,10 @@
       <c r="C32" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="108" t="s">
+      <c r="D32" s="98" t="s">
         <v>66</v>
       </c>
-      <c r="E32" s="109"/>
+      <c r="E32" s="99"/>
     </row>
     <row r="33" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21">
@@ -2963,10 +2963,10 @@
       <c r="C33" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="108" t="s">
+      <c r="D33" s="98" t="s">
         <v>66</v>
       </c>
-      <c r="E33" s="109"/>
+      <c r="E33" s="99"/>
     </row>
     <row r="34" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21">
@@ -2978,10 +2978,10 @@
       <c r="C34" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="108" t="s">
+      <c r="D34" s="98" t="s">
         <v>66</v>
       </c>
-      <c r="E34" s="109"/>
+      <c r="E34" s="99"/>
     </row>
     <row r="35" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="21">
@@ -2993,10 +2993,10 @@
       <c r="C35" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="D35" s="104" t="s">
+      <c r="D35" s="94" t="s">
         <v>72</v>
       </c>
-      <c r="E35" s="105"/>
+      <c r="E35" s="95"/>
     </row>
     <row r="36" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="21">
@@ -3008,10 +3008,10 @@
       <c r="C36" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="104" t="s">
+      <c r="D36" s="94" t="s">
         <v>72</v>
       </c>
-      <c r="E36" s="105"/>
+      <c r="E36" s="95"/>
     </row>
     <row r="37" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="73">
@@ -3023,10 +3023,10 @@
       <c r="C37" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="D37" s="104" t="s">
+      <c r="D37" s="94" t="s">
         <v>72</v>
       </c>
-      <c r="E37" s="105"/>
+      <c r="E37" s="95"/>
     </row>
     <row r="38" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="31">
@@ -3038,10 +3038,10 @@
       <c r="C38" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="D38" s="104" t="s">
+      <c r="D38" s="94" t="s">
         <v>72</v>
       </c>
-      <c r="E38" s="105"/>
+      <c r="E38" s="95"/>
     </row>
     <row r="39" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="78">
@@ -3053,10 +3053,10 @@
       <c r="C39" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="D39" s="110" t="s">
+      <c r="D39" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="E39" s="111"/>
+      <c r="E39" s="93"/>
     </row>
     <row r="40" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="21">
@@ -3068,10 +3068,10 @@
       <c r="C40" s="77" t="s">
         <v>74</v>
       </c>
-      <c r="D40" s="110" t="s">
+      <c r="D40" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="E40" s="111"/>
+      <c r="E40" s="93"/>
     </row>
     <row r="41" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="21">
@@ -3083,10 +3083,10 @@
       <c r="C41" s="77" t="s">
         <v>74</v>
       </c>
-      <c r="D41" s="110" t="s">
+      <c r="D41" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="E41" s="111"/>
+      <c r="E41" s="93"/>
     </row>
     <row r="42" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="21">
@@ -3098,10 +3098,10 @@
       <c r="C42" s="77" t="s">
         <v>74</v>
       </c>
-      <c r="D42" s="110" t="s">
+      <c r="D42" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="E42" s="111"/>
+      <c r="E42" s="93"/>
     </row>
     <row r="43" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="21">
@@ -3113,10 +3113,10 @@
       <c r="C43" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="D43" s="110" t="s">
+      <c r="D43" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="E43" s="111"/>
+      <c r="E43" s="93"/>
     </row>
     <row r="44" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="73">
@@ -3128,20 +3128,39 @@
       <c r="C44" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="D44" s="110" t="s">
+      <c r="D44" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="E44" s="111"/>
+      <c r="E44" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="D27:E27"/>
@@ -3154,32 +3173,13 @@
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3189,7 +3189,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC65C15-1C40-4251-A583-2703229E8E4D}">
   <dimension ref="A1:F204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Degrees HAY and GGS added
</commit_message>
<xml_diff>
--- a/test/xlsx/tablas_referencia.xlsx
+++ b/test/xlsx/tablas_referencia.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorena/Documents/GitHub/rails_projects/rptconsultants/test/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF774D5-BCB1-9444-9AAF-8C81DD5C73B0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5511C87B-A911-BB4A-B90C-1F9FE74F9E89}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{44D62DAF-BDC8-487B-86CE-15C7037211D0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{44D62DAF-BDC8-487B-86CE-15C7037211D0}"/>
   </bookViews>
   <sheets>
     <sheet name="grado" sheetId="1" r:id="rId1"/>
     <sheet name="roles" sheetId="2" r:id="rId2"/>
     <sheet name="criterio" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="264">
   <si>
     <t>grado</t>
   </si>
@@ -821,6 +821,12 @@
   </si>
   <si>
     <t>tipo_id</t>
+  </si>
+  <si>
+    <t>hay</t>
+  </si>
+  <si>
+    <t>ggs</t>
   </si>
 </sst>
 </file>
@@ -1541,7 +1547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1816,66 +1822,70 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2190,15 +2200,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ACB500F-32B4-40AA-B405-375E0A1D7B06}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2211,8 +2221,14 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="112" t="s">
+        <v>262</v>
+      </c>
+      <c r="F1" s="112" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>18</v>
       </c>
@@ -2225,8 +2241,16 @@
       <c r="D2" s="8">
         <v>3016</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="113">
+        <f>A2+8</f>
+        <v>26</v>
+      </c>
+      <c r="F2" s="113">
+        <f>A2+3</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9">
         <v>17</v>
       </c>
@@ -2239,8 +2263,16 @@
       <c r="D3" s="12">
         <v>2408</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="113">
+        <f t="shared" ref="E3:E19" si="0">A3+8</f>
+        <v>25</v>
+      </c>
+      <c r="F3" s="113">
+        <f t="shared" ref="F3:F19" si="1">A3+3</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>16</v>
       </c>
@@ -2253,8 +2285,16 @@
       <c r="D4" s="16">
         <v>1807</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="113">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="F4" s="113">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <v>15</v>
       </c>
@@ -2267,8 +2307,16 @@
       <c r="D5" s="12">
         <v>1468</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="113">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="F5" s="113">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>14</v>
       </c>
@@ -2281,8 +2329,16 @@
       <c r="D6" s="16">
         <v>1077</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="113">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="F6" s="113">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>13</v>
       </c>
@@ -2295,8 +2351,16 @@
       <c r="D7" s="12">
         <v>902</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="113">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="F7" s="113">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>12</v>
       </c>
@@ -2309,8 +2373,16 @@
       <c r="D8" s="16">
         <v>757</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="113">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F8" s="113">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>11</v>
       </c>
@@ -2323,8 +2395,16 @@
       <c r="D9" s="12">
         <v>633</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="113">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F9" s="113">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <v>10</v>
       </c>
@@ -2337,8 +2417,16 @@
       <c r="D10" s="16">
         <v>532</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="113">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F10" s="113">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -2351,8 +2439,16 @@
       <c r="D11" s="12">
         <v>445</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="113">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="F11" s="113">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="13">
         <v>8</v>
       </c>
@@ -2365,8 +2461,16 @@
       <c r="D12" s="16">
         <v>374</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="113">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F12" s="113">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <v>7</v>
       </c>
@@ -2379,8 +2483,16 @@
       <c r="D13" s="12">
         <v>312</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="113">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F13" s="113">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="13">
         <v>6</v>
       </c>
@@ -2393,8 +2505,16 @@
       <c r="D14" s="16">
         <v>263</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="113">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="F14" s="113">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <v>5</v>
       </c>
@@ -2407,8 +2527,16 @@
       <c r="D15" s="12">
         <v>220</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="113">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F15" s="113">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="13">
         <v>4</v>
       </c>
@@ -2421,8 +2549,16 @@
       <c r="D16" s="16">
         <v>185</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="113">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F16" s="113">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
         <v>3</v>
       </c>
@@ -2435,8 +2571,16 @@
       <c r="D17" s="12">
         <v>154</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="113">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F17" s="113">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="13">
         <v>2</v>
       </c>
@@ -2449,8 +2593,16 @@
       <c r="D18" s="16">
         <v>129</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="113">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F18" s="113">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>1</v>
       </c>
@@ -2462,6 +2614,14 @@
       </c>
       <c r="D19" s="20">
         <v>108</v>
+      </c>
+      <c r="E19" s="113">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F19" s="113">
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2473,7 +2633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575881AF-8C00-4C5E-94D1-79C6F03A8C05}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C12" sqref="C12:C13"/>
     </sheetView>
   </sheetViews>
@@ -2496,7 +2656,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21">
         <v>7</v>
       </c>
@@ -2506,12 +2666,12 @@
       <c r="C2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="106" t="s">
+      <c r="D2" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="107"/>
-    </row>
-    <row r="3" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="93"/>
+    </row>
+    <row r="3" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <v>6</v>
       </c>
@@ -2521,12 +2681,12 @@
       <c r="C3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="106" t="s">
+      <c r="D3" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="107"/>
-    </row>
-    <row r="4" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="93"/>
+    </row>
+    <row r="4" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <v>5</v>
       </c>
@@ -2536,10 +2696,10 @@
       <c r="C4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="106" t="s">
+      <c r="D4" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="107"/>
+      <c r="E4" s="93"/>
     </row>
     <row r="5" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26">
@@ -2551,12 +2711,12 @@
       <c r="C5" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="106" t="s">
+      <c r="D5" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="107"/>
-    </row>
-    <row r="6" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="93"/>
+    </row>
+    <row r="6" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29">
         <v>4</v>
       </c>
@@ -2566,10 +2726,10 @@
       <c r="C6" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="106" t="s">
+      <c r="D6" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="107"/>
+      <c r="E6" s="93"/>
     </row>
     <row r="7" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26">
@@ -2581,12 +2741,12 @@
       <c r="C7" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="106" t="s">
+      <c r="D7" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="107"/>
-    </row>
-    <row r="8" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="93"/>
+    </row>
+    <row r="8" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31">
         <v>3</v>
       </c>
@@ -2596,12 +2756,12 @@
       <c r="C8" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="106" t="s">
+      <c r="D8" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="107"/>
-    </row>
-    <row r="9" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="93"/>
+    </row>
+    <row r="9" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
         <v>3</v>
       </c>
@@ -2611,12 +2771,12 @@
       <c r="C9" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="106" t="s">
+      <c r="D9" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="107"/>
-    </row>
-    <row r="10" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="93"/>
+    </row>
+    <row r="10" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <v>2</v>
       </c>
@@ -2626,12 +2786,12 @@
       <c r="C10" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="106" t="s">
+      <c r="D10" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="107"/>
-    </row>
-    <row r="11" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="93"/>
+    </row>
+    <row r="11" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
         <v>5</v>
       </c>
@@ -2641,38 +2801,38 @@
       <c r="C11" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="102" t="s">
+      <c r="D11" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="103"/>
+      <c r="E11" s="99"/>
     </row>
     <row r="12" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
         <v>4</v>
       </c>
-      <c r="B12" s="108" t="s">
+      <c r="B12" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="110" t="s">
+      <c r="C12" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="102" t="s">
+      <c r="D12" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="103"/>
+      <c r="E12" s="99"/>
     </row>
     <row r="13" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29">
         <v>4</v>
       </c>
-      <c r="B13" s="109"/>
-      <c r="C13" s="111"/>
-      <c r="D13" s="102" t="s">
+      <c r="B13" s="95"/>
+      <c r="C13" s="97"/>
+      <c r="D13" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="103"/>
-    </row>
-    <row r="14" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="99"/>
+    </row>
+    <row r="14" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
         <v>3</v>
       </c>
@@ -2682,10 +2842,10 @@
       <c r="C14" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="102" t="s">
+      <c r="D14" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="103"/>
+      <c r="E14" s="99"/>
     </row>
     <row r="15" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31">
@@ -2693,12 +2853,12 @@
       </c>
       <c r="B15" s="37"/>
       <c r="C15" s="38"/>
-      <c r="D15" s="102" t="s">
+      <c r="D15" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="103"/>
-    </row>
-    <row r="16" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="99"/>
+    </row>
+    <row r="16" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
         <v>3</v>
       </c>
@@ -2708,12 +2868,12 @@
       <c r="C16" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="102" t="s">
+      <c r="D16" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="103"/>
-    </row>
-    <row r="17" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="99"/>
+    </row>
+    <row r="17" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21">
         <v>2</v>
       </c>
@@ -2723,10 +2883,10 @@
       <c r="C17" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="102" t="s">
+      <c r="D17" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="103"/>
+      <c r="E17" s="99"/>
     </row>
     <row r="18" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="45">
@@ -2738,12 +2898,12 @@
       <c r="C18" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="102" t="s">
+      <c r="D18" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="103"/>
-    </row>
-    <row r="19" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="99"/>
+    </row>
+    <row r="19" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="45">
         <v>8</v>
       </c>
@@ -2753,12 +2913,12 @@
       <c r="C19" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="104" t="s">
+      <c r="D19" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="105"/>
-    </row>
-    <row r="20" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="103"/>
+    </row>
+    <row r="20" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21">
         <v>7</v>
       </c>
@@ -2768,12 +2928,12 @@
       <c r="C20" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="104" t="s">
+      <c r="D20" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="105"/>
-    </row>
-    <row r="21" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="103"/>
+    </row>
+    <row r="21" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21">
         <v>6</v>
       </c>
@@ -2783,12 +2943,12 @@
       <c r="C21" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="104" t="s">
+      <c r="D21" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="105"/>
-    </row>
-    <row r="22" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="103"/>
+    </row>
+    <row r="22" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21">
         <v>5</v>
       </c>
@@ -2798,12 +2958,12 @@
       <c r="C22" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="104" t="s">
+      <c r="D22" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="105"/>
-    </row>
-    <row r="23" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E22" s="103"/>
+    </row>
+    <row r="23" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21">
         <v>11</v>
       </c>
@@ -2818,7 +2978,7 @@
       </c>
       <c r="E23" s="101"/>
     </row>
-    <row r="24" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21">
         <v>10</v>
       </c>
@@ -2833,7 +2993,7 @@
       </c>
       <c r="E24" s="101"/>
     </row>
-    <row r="25" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="21">
         <v>9</v>
       </c>
@@ -2858,10 +3018,10 @@
       <c r="C26" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="96" t="s">
+      <c r="D26" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="97"/>
+      <c r="E26" s="107"/>
     </row>
     <row r="27" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="45">
@@ -2873,12 +3033,12 @@
       <c r="C27" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="96" t="s">
+      <c r="D27" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="97"/>
-    </row>
-    <row r="28" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="107"/>
+    </row>
+    <row r="28" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="21">
         <v>7</v>
       </c>
@@ -2888,12 +3048,12 @@
       <c r="C28" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="D28" s="96" t="s">
+      <c r="D28" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="97"/>
-    </row>
-    <row r="29" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E28" s="107"/>
+    </row>
+    <row r="29" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="21">
         <v>6</v>
       </c>
@@ -2903,12 +3063,12 @@
       <c r="C29" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="96" t="s">
+      <c r="D29" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="97"/>
-    </row>
-    <row r="30" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E29" s="107"/>
+    </row>
+    <row r="30" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="21">
         <v>5</v>
       </c>
@@ -2918,10 +3078,10 @@
       <c r="C30" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="96" t="s">
+      <c r="D30" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="97"/>
+      <c r="E30" s="107"/>
     </row>
     <row r="31" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="31">
@@ -2933,10 +3093,10 @@
       <c r="C31" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="98" t="s">
+      <c r="D31" s="108" t="s">
         <v>66</v>
       </c>
-      <c r="E31" s="99"/>
+      <c r="E31" s="109"/>
     </row>
     <row r="32" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="21">
@@ -2948,10 +3108,10 @@
       <c r="C32" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="98" t="s">
+      <c r="D32" s="108" t="s">
         <v>66</v>
       </c>
-      <c r="E32" s="99"/>
+      <c r="E32" s="109"/>
     </row>
     <row r="33" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21">
@@ -2963,10 +3123,10 @@
       <c r="C33" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="98" t="s">
+      <c r="D33" s="108" t="s">
         <v>66</v>
       </c>
-      <c r="E33" s="99"/>
+      <c r="E33" s="109"/>
     </row>
     <row r="34" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21">
@@ -2978,10 +3138,10 @@
       <c r="C34" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="98" t="s">
+      <c r="D34" s="108" t="s">
         <v>66</v>
       </c>
-      <c r="E34" s="99"/>
+      <c r="E34" s="109"/>
     </row>
     <row r="35" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="21">
@@ -2993,10 +3153,10 @@
       <c r="C35" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="D35" s="94" t="s">
+      <c r="D35" s="104" t="s">
         <v>72</v>
       </c>
-      <c r="E35" s="95"/>
+      <c r="E35" s="105"/>
     </row>
     <row r="36" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="21">
@@ -3008,10 +3168,10 @@
       <c r="C36" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="94" t="s">
+      <c r="D36" s="104" t="s">
         <v>72</v>
       </c>
-      <c r="E36" s="95"/>
+      <c r="E36" s="105"/>
     </row>
     <row r="37" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="73">
@@ -3023,10 +3183,10 @@
       <c r="C37" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="D37" s="94" t="s">
+      <c r="D37" s="104" t="s">
         <v>72</v>
       </c>
-      <c r="E37" s="95"/>
+      <c r="E37" s="105"/>
     </row>
     <row r="38" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="31">
@@ -3038,10 +3198,10 @@
       <c r="C38" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="D38" s="94" t="s">
+      <c r="D38" s="104" t="s">
         <v>72</v>
       </c>
-      <c r="E38" s="95"/>
+      <c r="E38" s="105"/>
     </row>
     <row r="39" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="78">
@@ -3053,10 +3213,10 @@
       <c r="C39" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="D39" s="92" t="s">
+      <c r="D39" s="110" t="s">
         <v>81</v>
       </c>
-      <c r="E39" s="93"/>
+      <c r="E39" s="111"/>
     </row>
     <row r="40" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="21">
@@ -3068,12 +3228,12 @@
       <c r="C40" s="77" t="s">
         <v>74</v>
       </c>
-      <c r="D40" s="92" t="s">
+      <c r="D40" s="110" t="s">
         <v>81</v>
       </c>
-      <c r="E40" s="93"/>
-    </row>
-    <row r="41" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E40" s="111"/>
+    </row>
+    <row r="41" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="21">
         <v>16</v>
       </c>
@@ -3083,12 +3243,12 @@
       <c r="C41" s="77" t="s">
         <v>74</v>
       </c>
-      <c r="D41" s="92" t="s">
+      <c r="D41" s="110" t="s">
         <v>81</v>
       </c>
-      <c r="E41" s="93"/>
-    </row>
-    <row r="42" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E41" s="111"/>
+    </row>
+    <row r="42" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="21">
         <v>15</v>
       </c>
@@ -3098,10 +3258,10 @@
       <c r="C42" s="77" t="s">
         <v>74</v>
       </c>
-      <c r="D42" s="92" t="s">
+      <c r="D42" s="110" t="s">
         <v>81</v>
       </c>
-      <c r="E42" s="93"/>
+      <c r="E42" s="111"/>
     </row>
     <row r="43" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="21">
@@ -3113,10 +3273,10 @@
       <c r="C43" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="D43" s="92" t="s">
+      <c r="D43" s="110" t="s">
         <v>81</v>
       </c>
-      <c r="E43" s="93"/>
+      <c r="E43" s="111"/>
     </row>
     <row r="44" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="73">
@@ -3128,27 +3288,32 @@
       <c r="C44" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="D44" s="92" t="s">
+      <c r="D44" s="110" t="s">
         <v>81</v>
       </c>
-      <c r="E44" s="93"/>
+      <c r="E44" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
@@ -3161,25 +3326,20 @@
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>